<commit_message>
create flight and out all flight
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CheckIn.xlsx
+++ b/src/main/resources/input_excel_file/booking/CheckIn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Check_In_Bag" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="136">
   <si>
     <t>tc_id</t>
   </si>
@@ -151,7 +151,7 @@
     <t>assert_bag</t>
   </si>
   <si>
-    <t>CI_001</t>
+    <t>CI_PLAYER1_001</t>
   </si>
   <si>
     <t>VST_Kiểm tra check in bag</t>
@@ -178,115 +178,256 @@
     <t>{{CTX:GUEST_STYLE_NAME_0}}</t>
   </si>
   <si>
+    <t>{{CTX:BOOKING_DATE_0}}</t>
+  </si>
+  <si>
+    <t>{{CTX:COURSE_TYPE_0}}</t>
+  </si>
+  <si>
+    <t>{{CTX:TEE_TYPE_0}}</t>
+  </si>
+  <si>
+    <t>{{CTX:CUSTOMER_NAME_0}}</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>{{CTX:FULL_NAME}}</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>check_in_bag_expect.json</t>
+  </si>
+  <si>
+    <t>NOT_NULL</t>
+  </si>
+  <si>
+    <t>WAITING</t>
+  </si>
+  <si>
+    <t>CI_PLAYER1_002</t>
+  </si>
+  <si>
+    <t>MB_Kiểm tra check in bag</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_UID_OF_GUEST_0}}</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_CARD_UID_0}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER1_003</t>
+  </si>
+  <si>
+    <t>MBG_Kiểm tra check in bag</t>
+  </si>
+  <si>
+    <t>CI_PLAYER1_004</t>
+  </si>
+  <si>
+    <t>NG_Kiểm tra check in bag</t>
+  </si>
+  <si>
+    <t>CI_PLAYER1_005</t>
+  </si>
+  <si>
+    <t>AG_Kiểm tra check in bag</t>
+  </si>
+  <si>
+    <t>check_in_bag_agency_request.json</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>CI_PLAYER2_001</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_UID_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:HOLE_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_NAME_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_DATE_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:COURSE_TYPE_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:TEE_TYPE_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:CUSTOMER_NAME_1}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER2_002</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_UID_OF_GUEST_1}}</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_CARD_UID_1}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER2_003</t>
+  </si>
+  <si>
+    <t>CI_PLAYER2_004</t>
+  </si>
+  <si>
+    <t>CI_PLAYER2_005</t>
+  </si>
+  <si>
+    <t>CI_PLAYER3_001</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_UID_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:HOLE_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_NAME_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_DATE_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:COURSE_TYPE_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:TEE_TYPE_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:CUSTOMER_NAME_2}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER3_002</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_UID_OF_GUEST_2}}</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_CARD_UID_2}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER3_003</t>
+  </si>
+  <si>
+    <t>CI_PLAYER3_004</t>
+  </si>
+  <si>
+    <t>CI_PLAYER3_005</t>
+  </si>
+  <si>
+    <t>CI_PLAYER4_001</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_UID_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:HOLE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_NAME_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_DATE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:COURSE_TYPE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:TEE_TYPE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:CUSTOMER_NAME_3}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER4_002</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_UID_OF_GUEST_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_CARD_UID_3}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER4_003</t>
+  </si>
+  <si>
+    <t>CI_PLAYER4_004</t>
+  </si>
+  <si>
+    <t>CI_PLAYER4_005</t>
+  </si>
+  <si>
+    <t>UCI_001</t>
+  </si>
+  <si>
+    <t>undo_check_in_bag_request.json</t>
+  </si>
+  <si>
+    <t>{{CTX:BAG}}</t>
+  </si>
+  <si>
+    <t>undo_check_in_bag_expect.json</t>
+  </si>
+  <si>
+    <t>check_sum</t>
+  </si>
+  <si>
+    <t>partner_uid</t>
+  </si>
+  <si>
+    <t>course_uid</t>
+  </si>
+  <si>
+    <t>assert_code</t>
+  </si>
+  <si>
+    <t>assert_desc</t>
+  </si>
+  <si>
+    <t>CI_EKYC_001</t>
+  </si>
+  <si>
+    <t>check_in_ekyc_request.json</t>
+  </si>
+  <si>
+    <t>{{CHECKSUM}}</t>
+  </si>
+  <si>
+    <t>{{CTX:PARTNER_UID}}</t>
+  </si>
+  <si>
+    <t>{{CTX:COURSE_UID}}</t>
+  </si>
+  <si>
     <t>{{TODAY}}</t>
-  </si>
-  <si>
-    <t>{{CTX:COURSE_TYPE_0}}</t>
-  </si>
-  <si>
-    <t>{{CTX:TEE_TYPE_0}}</t>
-  </si>
-  <si>
-    <t>{{CTX:CUSTOMER_NAME_0}}</t>
-  </si>
-  <si>
-    <t>CMS</t>
-  </si>
-  <si>
-    <t>MALE</t>
-  </si>
-  <si>
-    <t>{{CTX:FULL_NAME}}</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>check_in_bag_expect.json</t>
-  </si>
-  <si>
-    <t>NOT_NULL</t>
-  </si>
-  <si>
-    <t>WAITING</t>
-  </si>
-  <si>
-    <t>CI_002</t>
-  </si>
-  <si>
-    <t>MB_Kiểm tra check in bag</t>
-  </si>
-  <si>
-    <t>{{CTX:MEMBER_UID_OF_GUEST_0}}</t>
-  </si>
-  <si>
-    <t>{{CTX:MEMBER_CARD_UID_0}}</t>
-  </si>
-  <si>
-    <t>CI_003</t>
-  </si>
-  <si>
-    <t>MBG_Kiểm tra check in bag</t>
-  </si>
-  <si>
-    <t>CI_004</t>
-  </si>
-  <si>
-    <t>NG_Kiểm tra check in bag</t>
-  </si>
-  <si>
-    <t>CI_005</t>
-  </si>
-  <si>
-    <t>AG_Kiểm tra check in bag</t>
-  </si>
-  <si>
-    <t>check_in_bag_agency_request.json</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>UCI_001</t>
-  </si>
-  <si>
-    <t>undo_check_in_bag_request.json</t>
-  </si>
-  <si>
-    <t>{{CTX:BAG}}</t>
-  </si>
-  <si>
-    <t>undo_check_in_bag_expect.json</t>
-  </si>
-  <si>
-    <t>check_sum</t>
-  </si>
-  <si>
-    <t>partner_uid</t>
-  </si>
-  <si>
-    <t>course_uid</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>desc</t>
-  </si>
-  <si>
-    <t>check_in_ekyc_request.json</t>
-  </si>
-  <si>
-    <t>4f8fcfb05a1552d4c6cf399717845d94da3d29a2b198b5a24043feb4c98e768e</t>
-  </si>
-  <si>
-    <t>{{CTX:PARTNER_UID}}</t>
-  </si>
-  <si>
-    <t>{{CTX:COURSE_UID}}</t>
   </si>
   <si>
     <t>check_in_ekyc_expect.json</t>
@@ -505,12 +646,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -523,7 +658,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,70 +1136,70 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1597,17 +1738,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AN21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.7142857142857" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.8571428571429" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.9333333333333" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7904761904762" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
@@ -1622,12 +1763,13 @@
     <col min="16" max="16" width="17.8380952380952" style="13" customWidth="1"/>
     <col min="17" max="18" width="17.8380952380952" style="1" customWidth="1"/>
     <col min="19" max="19" width="21.1428571428571" style="13" customWidth="1"/>
-    <col min="20" max="27" width="24.7142857142857" style="1" customWidth="1"/>
-    <col min="28" max="28" width="24.7142857142857" style="13" customWidth="1"/>
-    <col min="29" max="30" width="24.7142857142857" style="1" customWidth="1"/>
-    <col min="31" max="33" width="24.7142857142857" style="13" customWidth="1"/>
-    <col min="34" max="34" width="24.7142857142857" style="1" customWidth="1"/>
-    <col min="35" max="35" width="22.8571428571429" style="13" customWidth="1"/>
+    <col min="20" max="21" width="24.7142857142857" style="1" customWidth="1"/>
+    <col min="22" max="27" width="12.7714285714286" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7714285714286" style="13" customWidth="1"/>
+    <col min="29" max="30" width="12.7714285714286" style="1" customWidth="1"/>
+    <col min="31" max="33" width="12.7714285714286" style="13" customWidth="1"/>
+    <col min="34" max="34" width="12.7714285714286" style="1" customWidth="1"/>
+    <col min="35" max="35" width="12.7714285714286" style="13" customWidth="1"/>
     <col min="36" max="36" width="31.4285714285714" style="1" customWidth="1"/>
     <col min="37" max="37" width="15.2857142857143" style="1" customWidth="1"/>
     <col min="38" max="38" width="20.8571428571429" style="1" customWidth="1"/>
@@ -1704,46 +1846,46 @@
       <c r="U1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AA1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AC1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AD1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AE1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="19" t="s">
         <v>32</v>
       </c>
       <c r="AH1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="22" t="s">
+      <c r="AI1" s="23" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="8" t="s">
@@ -1752,13 +1894,13 @@
       <c r="AK1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="23" t="s">
+      <c r="AL1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="23" t="s">
+      <c r="AM1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="23" t="s">
+      <c r="AN1" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1778,10 +1920,10 @@
       <c r="E2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="10">
         <v>100</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -1790,10 +1932,10 @@
       <c r="I2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10" t="s">
         <v>49</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -1805,13 +1947,13 @@
       <c r="N2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="12">
-        <v>0</v>
-      </c>
-      <c r="P2" s="12" t="s">
+      <c r="O2" s="10">
+        <v>0</v>
+      </c>
+      <c r="P2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="10" t="s">
         <v>54</v>
       </c>
       <c r="R2" s="4" t="s">
@@ -1820,23 +1962,23 @@
       <c r="S2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="12">
-        <v>0</v>
-      </c>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="12" t="s">
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10">
+        <v>0</v>
+      </c>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="10" t="s">
         <v>56</v>
       </c>
       <c r="AI2" s="21" t="s">
@@ -1851,11 +1993,11 @@
       <c r="AL2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AM2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AN2" s="15">
-        <f>G2</f>
+      <c r="AN2" s="10">
+        <f t="shared" ref="AN2:AN21" si="0">G2</f>
         <v>100</v>
       </c>
     </row>
@@ -1875,10 +2017,10 @@
       <c r="E3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="10">
         <f>G2+1</f>
         <v>101</v>
       </c>
@@ -1888,10 +2030,10 @@
       <c r="I3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="10" t="s">
         <v>49</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -1903,13 +2045,13 @@
       <c r="N3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="12">
-        <v>0</v>
-      </c>
-      <c r="P3" s="12" t="s">
+      <c r="O3" s="10">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="10" t="s">
         <v>54</v>
       </c>
       <c r="R3" s="4" t="s">
@@ -1918,27 +2060,27 @@
       <c r="S3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="V3" s="12">
-        <v>0</v>
-      </c>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="12" t="s">
+      <c r="V3" s="10">
+        <v>0</v>
+      </c>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="10" t="s">
         <v>56</v>
       </c>
       <c r="AI3" s="21" t="s">
@@ -1953,11 +2095,11 @@
       <c r="AL3" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AM3" s="15" t="s">
+      <c r="AM3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AN3" s="15">
-        <f>G3</f>
+      <c r="AN3" s="10">
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
     </row>
@@ -1977,11 +2119,11 @@
       <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="12">
-        <f>G3+1</f>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G16" si="1">G3+1</f>
         <v>102</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -1990,10 +2132,10 @@
       <c r="I4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="10" t="s">
         <v>49</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -2005,13 +2147,13 @@
       <c r="N4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="12">
-        <v>0</v>
-      </c>
-      <c r="P4" s="12" t="s">
+      <c r="O4" s="10">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="10" t="s">
         <v>54</v>
       </c>
       <c r="R4" s="4" t="s">
@@ -2020,11 +2162,11 @@
       <c r="S4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="T4" s="10" t="s">
         <v>63</v>
       </c>
       <c r="U4" s="10"/>
-      <c r="V4" s="12">
+      <c r="V4" s="10">
         <v>0</v>
       </c>
       <c r="W4" s="10"/>
@@ -2032,13 +2174,13 @@
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
       <c r="AA4" s="10"/>
-      <c r="AB4" s="20"/>
+      <c r="AB4" s="21"/>
       <c r="AC4" s="10"/>
       <c r="AD4" s="10"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="12" t="s">
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="10" t="s">
         <v>56</v>
       </c>
       <c r="AI4" s="21" t="s">
@@ -2053,11 +2195,11 @@
       <c r="AL4" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AM4" s="15" t="s">
+      <c r="AM4" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AN4" s="15">
-        <f>G4</f>
+      <c r="AN4" s="10">
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
     </row>
@@ -2077,11 +2219,11 @@
       <c r="E5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="12">
-        <f>G4+1</f>
+      <c r="G5" s="10">
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -2090,10 +2232,10 @@
       <c r="I5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="10" t="s">
         <v>49</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -2105,13 +2247,13 @@
       <c r="N5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="12">
-        <v>0</v>
-      </c>
-      <c r="P5" s="12" t="s">
+      <c r="O5" s="10">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="10" t="s">
         <v>54</v>
       </c>
       <c r="R5" s="4" t="s">
@@ -2122,7 +2264,7 @@
       </c>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
-      <c r="V5" s="12">
+      <c r="V5" s="10">
         <v>0</v>
       </c>
       <c r="W5" s="10"/>
@@ -2130,13 +2272,13 @@
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
       <c r="AA5" s="10"/>
-      <c r="AB5" s="20"/>
+      <c r="AB5" s="21"/>
       <c r="AC5" s="10"/>
       <c r="AD5" s="10"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="12" t="s">
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="10" t="s">
         <v>56</v>
       </c>
       <c r="AI5" s="21" t="s">
@@ -2151,11 +2293,11 @@
       <c r="AL5" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AM5" s="15" t="s">
+      <c r="AM5" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AN5" s="15">
-        <f>G5</f>
+      <c r="AN5" s="10">
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
     </row>
@@ -2175,11 +2317,11 @@
       <c r="E6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="12">
-        <f>G5+1</f>
+      <c r="G6" s="10">
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -2188,10 +2330,10 @@
       <c r="I6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="10" t="s">
         <v>49</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -2203,13 +2345,13 @@
       <c r="N6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="12">
-        <v>0</v>
-      </c>
-      <c r="P6" s="12" t="s">
+      <c r="O6" s="10">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="10" t="s">
         <v>54</v>
       </c>
       <c r="R6" s="4" t="s">
@@ -2220,31 +2362,31 @@
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
-      <c r="V6" s="12">
+      <c r="V6" s="10">
         <v>378</v>
       </c>
-      <c r="W6" s="12">
+      <c r="W6" s="10">
         <v>1600000</v>
       </c>
-      <c r="X6" s="12">
+      <c r="X6" s="10">
         <v>400000</v>
       </c>
-      <c r="Y6" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="12">
+      <c r="Y6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="10">
         <v>0</v>
       </c>
       <c r="AB6" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AC6" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="12">
+      <c r="AC6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="10">
         <v>0</v>
       </c>
       <c r="AE6" s="21" t="s">
@@ -2256,7 +2398,7 @@
       <c r="AG6" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AH6" s="12" t="s">
+      <c r="AH6" s="10" t="s">
         <v>56</v>
       </c>
       <c r="AI6" s="21" t="s">
@@ -2271,12 +2413,1566 @@
       <c r="AL6" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AM6" s="15" t="s">
+      <c r="AM6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AN6" s="15">
-        <f>G6</f>
+      <c r="AN6" s="10">
+        <f t="shared" si="0"/>
         <v>104</v>
+      </c>
+    </row>
+    <row r="7" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A7" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="16">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16">
+        <v>0</v>
+      </c>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="22"/>
+      <c r="AG7" s="22"/>
+      <c r="AH7" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK7" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL7" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN7" s="16">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A8" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="16">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="U8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="V8" s="16">
+        <v>0</v>
+      </c>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="22"/>
+      <c r="AH8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI8" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK8" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN8" s="16">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A9" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="16">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16">
+        <v>0</v>
+      </c>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI9" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK9" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM9" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN9" s="16">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A10" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16">
+        <v>0</v>
+      </c>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="16"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI10" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK10" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN10" s="16">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A11" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16">
+        <v>378</v>
+      </c>
+      <c r="W11" s="16">
+        <v>1600000</v>
+      </c>
+      <c r="X11" s="16">
+        <v>400000</v>
+      </c>
+      <c r="Y11" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC11" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF11" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG11" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI11" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK11" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL11" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN11" s="16">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" ref="G12:G21" si="2">G11+1</f>
+        <v>110</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O12" s="10">
+        <v>0</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10">
+        <v>0</v>
+      </c>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="21"/>
+      <c r="AF12" s="21"/>
+      <c r="AG12" s="21"/>
+      <c r="AH12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI12" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK12" s="10">
+        <v>200</v>
+      </c>
+      <c r="AL12" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN12" s="10">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O13" s="10">
+        <v>0</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="V13" s="10">
+        <v>0</v>
+      </c>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="21"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="21"/>
+      <c r="AG13" s="21"/>
+      <c r="AH13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI13" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK13" s="10">
+        <v>200</v>
+      </c>
+      <c r="AL13" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM13" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN13" s="10">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T14" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10">
+        <v>0</v>
+      </c>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="21"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="21"/>
+      <c r="AG14" s="21"/>
+      <c r="AH14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI14" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK14" s="10">
+        <v>200</v>
+      </c>
+      <c r="AL14" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN14" s="10">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="10">
+        <v>0</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10">
+        <v>0</v>
+      </c>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="21"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="21"/>
+      <c r="AF15" s="21"/>
+      <c r="AG15" s="21"/>
+      <c r="AH15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI15" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK15" s="10">
+        <v>200</v>
+      </c>
+      <c r="AL15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN15" s="10">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:40">
+      <c r="A16" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O16" s="10">
+        <v>0</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10">
+        <v>378</v>
+      </c>
+      <c r="W16" s="10">
+        <v>1600000</v>
+      </c>
+      <c r="X16" s="10">
+        <v>400000</v>
+      </c>
+      <c r="Y16" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK16" s="10">
+        <v>200</v>
+      </c>
+      <c r="AL16" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN16" s="10">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A17" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="16">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q17" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R17" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16">
+        <v>0</v>
+      </c>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="16"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI17" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK17" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN17" s="16">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A18" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="16">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R18" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="U18" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="V18" s="16">
+        <v>0</v>
+      </c>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="16"/>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="16"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+      <c r="AG18" s="22"/>
+      <c r="AH18" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI18" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ18" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK18" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN18" s="16">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A19" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="16">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0</v>
+      </c>
+      <c r="P19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R19" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T19" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16">
+        <v>0</v>
+      </c>
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="16"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="16"/>
+      <c r="AD19" s="16"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
+      <c r="AG19" s="22"/>
+      <c r="AH19" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI19" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ19" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK19" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL19" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM19" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN19" s="16">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A20" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="16">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16">
+        <v>0</v>
+      </c>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
+      <c r="AG20" s="22"/>
+      <c r="AH20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI20" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ20" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK20" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN20" s="16">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" s="12" customFormat="1" customHeight="1" spans="1:40">
+      <c r="A21" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="16">
+        <f>G20+1</f>
+        <v>119</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q21" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="R21" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16">
+        <v>378</v>
+      </c>
+      <c r="W21" s="16">
+        <v>1600000</v>
+      </c>
+      <c r="X21" s="16">
+        <v>400000</v>
+      </c>
+      <c r="Y21" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC21" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF21" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG21" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH21" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI21" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ21" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK21" s="16">
+        <v>200</v>
+      </c>
+      <c r="AL21" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM21" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN21" s="16">
+        <f t="shared" si="0"/>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2339,7 +4035,7 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>41</v>
@@ -2348,16 +4044,16 @@
         <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>75</v>
+      <c r="F2" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="H2" s="10">
         <v>200</v>
@@ -2374,8 +4070,8 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
@@ -2384,14 +4080,14 @@
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.4285714285714" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.8571428571429" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.7142857142857" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
     <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.14285714285714" style="1"/>
+    <col min="12" max="12" width="19.7142857142857" style="1" customWidth="1"/>
     <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
     <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
     <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
@@ -2412,13 +4108,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -2433,15 +4129,15 @@
         <v>36</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>62</v>
@@ -2450,34 +4146,34 @@
         <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="K2" s="10">
         <v>200</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fee of bag bill and add sub
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CheckIn.xlsx
+++ b/src/main/resources/input_excel_file/booking/CheckIn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="11460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Check_In_Bag_Player1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="143">
   <si>
     <t>tc_id</t>
   </si>
@@ -391,13 +391,34 @@
     <t>UCI_001</t>
   </si>
   <si>
+    <t>VST_Kiểm tra undo check in bag</t>
+  </si>
+  <si>
     <t>undo_check_in_bag_request.json</t>
   </si>
   <si>
-    <t>{{CTX:BAG}}</t>
+    <t>{{CTX:BAG_0}}</t>
   </si>
   <si>
     <t>undo_check_in_bag_expect.json</t>
+  </si>
+  <si>
+    <t>UCI_002</t>
+  </si>
+  <si>
+    <t>{{CTX:BAG_1}}</t>
+  </si>
+  <si>
+    <t>UCI_003</t>
+  </si>
+  <si>
+    <t>{{CTX:BAG_2}}</t>
+  </si>
+  <si>
+    <t>UCI_004</t>
+  </si>
+  <si>
+    <t>{{CTX:BAG_3}}</t>
   </si>
   <si>
     <t>check_sum</t>
@@ -1728,7 +1749,7 @@
   <sheetPr/>
   <dimension ref="A1:AN6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -4494,13 +4515,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="13.7142857142857" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
@@ -4548,24 +4569,102 @@
         <v>118</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="E3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="7">
         <v>200</v>
       </c>
     </row>
@@ -4618,13 +4717,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -4639,15 +4738,15 @@
         <v>36</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>62</v>
@@ -4656,34 +4755,34 @@
         <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="K2" s="7">
         <v>200</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
single payment list and check out
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CheckIn.xlsx
+++ b/src/main/resources/input_excel_file/booking/CheckIn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Check_In_Bag_Player1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,10 @@
     <sheet name="Check_In_Bag_Player3" sheetId="5" r:id="rId3"/>
     <sheet name="Check_In_Bag_Player4" sheetId="6" r:id="rId4"/>
     <sheet name="Undo_Check_In" sheetId="3" r:id="rId5"/>
-    <sheet name="Check_In_Ekyc" sheetId="2" r:id="rId6"/>
+    <sheet name="Check_In_Ekyc_Player1" sheetId="2" r:id="rId6"/>
+    <sheet name="Check_In_Ekyc_Player2" sheetId="7" r:id="rId7"/>
+    <sheet name="Check_In_Ekyc_Player3" sheetId="8" r:id="rId8"/>
+    <sheet name="Check_In_Ekyc_Player4" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="149">
   <si>
     <t>tc_id</t>
   </si>
@@ -486,10 +489,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -673,7 +676,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -695,12 +698,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1020,16 +1017,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1038,7 +1035,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1062,16 +1059,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1080,89 +1077,89 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1193,19 +1190,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1217,16 +1211,13 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1873,46 +1864,46 @@
       <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AA1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AE1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AG1" s="15" t="s">
         <v>32</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="18" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="8" t="s">
@@ -1999,16 +1990,16 @@
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
-      <c r="AB2" s="20"/>
+      <c r="AB2" s="19"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
       <c r="AH2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AI2" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ2" s="5" t="s">
@@ -2017,7 +2008,7 @@
       <c r="AK2" s="7">
         <v>200</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AL2" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM2" s="7" t="s">
@@ -2101,16 +2092,16 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-      <c r="AB3" s="20"/>
+      <c r="AB3" s="19"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
       <c r="AH3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI3" s="20" t="s">
+      <c r="AI3" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ3" s="5" t="s">
@@ -2119,7 +2110,7 @@
       <c r="AK3" s="7">
         <v>200</v>
       </c>
-      <c r="AL3" s="21" t="s">
+      <c r="AL3" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM3" s="7" t="s">
@@ -2201,16 +2192,16 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
-      <c r="AB4" s="20"/>
+      <c r="AB4" s="19"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
       <c r="AH4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI4" s="20" t="s">
+      <c r="AI4" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ4" s="5" t="s">
@@ -2219,7 +2210,7 @@
       <c r="AK4" s="7">
         <v>200</v>
       </c>
-      <c r="AL4" s="21" t="s">
+      <c r="AL4" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM4" s="7" t="s">
@@ -2299,16 +2290,16 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
-      <c r="AB5" s="20"/>
+      <c r="AB5" s="19"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
       <c r="AH5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI5" s="20" t="s">
+      <c r="AI5" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ5" s="5" t="s">
@@ -2317,7 +2308,7 @@
       <c r="AK5" s="7">
         <v>200</v>
       </c>
-      <c r="AL5" s="21" t="s">
+      <c r="AL5" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM5" s="7" t="s">
@@ -2407,7 +2398,7 @@
       <c r="AA6" s="7">
         <v>0</v>
       </c>
-      <c r="AB6" s="20" t="s">
+      <c r="AB6" s="19" t="s">
         <v>72</v>
       </c>
       <c r="AC6" s="7">
@@ -2416,19 +2407,19 @@
       <c r="AD6" s="7">
         <v>0</v>
       </c>
-      <c r="AE6" s="20" t="s">
+      <c r="AE6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="AF6" s="20" t="s">
+      <c r="AF6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="AG6" s="20" t="s">
+      <c r="AG6" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AH6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI6" s="20" t="s">
+      <c r="AI6" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ6" s="5" t="s">
@@ -2437,7 +2428,7 @@
       <c r="AK6" s="7">
         <v>200</v>
       </c>
-      <c r="AL6" s="21" t="s">
+      <c r="AL6" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM6" s="7" t="s">
@@ -2460,7 +2451,7 @@
   <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="5"/>
@@ -2565,46 +2556,46 @@
       <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AA1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AE1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AG1" s="15" t="s">
         <v>32</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="18" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="8" t="s">
@@ -2624,518 +2615,518 @@
       </c>
     </row>
     <row r="2" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>200</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O2" s="14">
-        <v>0</v>
-      </c>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="13">
+        <v>0</v>
+      </c>
+      <c r="P2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14">
-        <v>0</v>
-      </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="14" t="s">
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13">
+        <v>0</v>
+      </c>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI2" s="18" t="s">
+      <c r="AI2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK2" s="14">
+      <c r="AK2" s="13">
         <v>200</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="AL2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AM2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN2" s="14">
+      <c r="AN2" s="13">
         <f>G2</f>
         <v>200</v>
       </c>
     </row>
     <row r="3" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <f>G2+1</f>
         <v>201</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="14">
-        <v>0</v>
-      </c>
-      <c r="P3" s="14" t="s">
+      <c r="O3" s="13">
+        <v>0</v>
+      </c>
+      <c r="P3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="U3" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="V3" s="14">
-        <v>0</v>
-      </c>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="14" t="s">
+      <c r="V3" s="13">
+        <v>0</v>
+      </c>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI3" s="18" t="s">
+      <c r="AI3" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AJ3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK3" s="14">
+      <c r="AK3" s="13">
         <v>200</v>
       </c>
-      <c r="AL3" s="14" t="s">
+      <c r="AL3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM3" s="14" t="s">
+      <c r="AM3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN3" s="14">
+      <c r="AN3" s="13">
         <f>G3</f>
         <v>201</v>
       </c>
     </row>
     <row r="4" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <f>G3+1</f>
         <v>202</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="14">
-        <v>0</v>
-      </c>
-      <c r="P4" s="14" t="s">
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14">
-        <v>0</v>
-      </c>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
-      <c r="AH4" s="14" t="s">
+      <c r="U4" s="13"/>
+      <c r="V4" s="13">
+        <v>0</v>
+      </c>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI4" s="18" t="s">
+      <c r="AI4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ4" s="12" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK4" s="14">
+      <c r="AK4" s="13">
         <v>200</v>
       </c>
-      <c r="AL4" s="14" t="s">
+      <c r="AL4" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM4" s="14" t="s">
+      <c r="AM4" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN4" s="14">
+      <c r="AN4" s="13">
         <f>G4</f>
         <v>202</v>
       </c>
     </row>
     <row r="5" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <f>G4+1</f>
         <v>203</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O5" s="14">
-        <v>0</v>
-      </c>
-      <c r="P5" s="14" t="s">
+      <c r="O5" s="13">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14">
-        <v>0</v>
-      </c>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="14" t="s">
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13">
+        <v>0</v>
+      </c>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI5" s="18" t="s">
+      <c r="AI5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ5" s="12" t="s">
+      <c r="AJ5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK5" s="14">
+      <c r="AK5" s="13">
         <v>200</v>
       </c>
-      <c r="AL5" s="14" t="s">
+      <c r="AL5" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM5" s="14" t="s">
+      <c r="AM5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN5" s="14">
+      <c r="AN5" s="13">
         <f>G5</f>
         <v>203</v>
       </c>
     </row>
     <row r="6" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f>G5+1</f>
         <v>204</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O6" s="14">
-        <v>0</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="O6" s="13">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="S6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14">
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13">
         <v>378</v>
       </c>
-      <c r="W6" s="14">
+      <c r="W6" s="13">
         <v>1600000</v>
       </c>
-      <c r="X6" s="14">
+      <c r="X6" s="13">
         <v>400000</v>
       </c>
-      <c r="Y6" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="18" t="s">
+      <c r="Y6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AC6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="18" t="s">
+      <c r="AC6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AF6" s="18" t="s">
+      <c r="AF6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AG6" s="18" t="s">
+      <c r="AG6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AH6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI6" s="18" t="s">
+      <c r="AI6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ6" s="12" t="s">
+      <c r="AJ6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK6" s="14">
+      <c r="AK6" s="13">
         <v>200</v>
       </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AL6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM6" s="14" t="s">
+      <c r="AM6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN6" s="14">
+      <c r="AN6" s="13">
         <f>G6</f>
         <v>204</v>
       </c>
@@ -3257,46 +3248,46 @@
       <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AA1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AE1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AG1" s="15" t="s">
         <v>32</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="18" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="8" t="s">
@@ -3383,16 +3374,16 @@
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
-      <c r="AB2" s="20"/>
+      <c r="AB2" s="19"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
       <c r="AH2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AI2" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ2" s="5" t="s">
@@ -3401,7 +3392,7 @@
       <c r="AK2" s="7">
         <v>200</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AL2" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM2" s="7" t="s">
@@ -3485,16 +3476,16 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-      <c r="AB3" s="20"/>
+      <c r="AB3" s="19"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
       <c r="AH3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI3" s="20" t="s">
+      <c r="AI3" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ3" s="5" t="s">
@@ -3503,7 +3494,7 @@
       <c r="AK3" s="7">
         <v>200</v>
       </c>
-      <c r="AL3" s="21" t="s">
+      <c r="AL3" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM3" s="7" t="s">
@@ -3585,16 +3576,16 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
-      <c r="AB4" s="20"/>
+      <c r="AB4" s="19"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
       <c r="AH4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI4" s="20" t="s">
+      <c r="AI4" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ4" s="5" t="s">
@@ -3603,7 +3594,7 @@
       <c r="AK4" s="7">
         <v>200</v>
       </c>
-      <c r="AL4" s="21" t="s">
+      <c r="AL4" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM4" s="7" t="s">
@@ -3683,16 +3674,16 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
-      <c r="AB5" s="20"/>
+      <c r="AB5" s="19"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
       <c r="AH5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI5" s="20" t="s">
+      <c r="AI5" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ5" s="5" t="s">
@@ -3701,7 +3692,7 @@
       <c r="AK5" s="7">
         <v>200</v>
       </c>
-      <c r="AL5" s="21" t="s">
+      <c r="AL5" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM5" s="7" t="s">
@@ -3791,7 +3782,7 @@
       <c r="AA6" s="7">
         <v>0</v>
       </c>
-      <c r="AB6" s="20" t="s">
+      <c r="AB6" s="19" t="s">
         <v>72</v>
       </c>
       <c r="AC6" s="7">
@@ -3800,19 +3791,19 @@
       <c r="AD6" s="7">
         <v>0</v>
       </c>
-      <c r="AE6" s="20" t="s">
+      <c r="AE6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="AF6" s="20" t="s">
+      <c r="AF6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="AG6" s="20" t="s">
+      <c r="AG6" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AH6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI6" s="20" t="s">
+      <c r="AI6" s="19" t="s">
         <v>57</v>
       </c>
       <c r="AJ6" s="5" t="s">
@@ -3821,7 +3812,7 @@
       <c r="AK6" s="7">
         <v>200</v>
       </c>
-      <c r="AL6" s="21" t="s">
+      <c r="AL6" s="13" t="s">
         <v>59</v>
       </c>
       <c r="AM6" s="7" t="s">
@@ -3843,8 +3834,8 @@
   <sheetPr/>
   <dimension ref="A1:AN6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="5"/>
@@ -3949,46 +3940,46 @@
       <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AA1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AE1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AG1" s="15" t="s">
         <v>32</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="18" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="8" t="s">
@@ -4008,518 +3999,518 @@
       </c>
     </row>
     <row r="2" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>400</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="14">
-        <v>0</v>
-      </c>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="13">
+        <v>0</v>
+      </c>
+      <c r="P2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14">
-        <v>0</v>
-      </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="14" t="s">
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13">
+        <v>0</v>
+      </c>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI2" s="18" t="s">
+      <c r="AI2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK2" s="14">
+      <c r="AK2" s="13">
         <v>200</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="AL2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AM2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN2" s="14">
+      <c r="AN2" s="13">
         <f>G2</f>
         <v>400</v>
       </c>
     </row>
     <row r="3" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <f>G2+1</f>
         <v>401</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="O3" s="14">
-        <v>0</v>
-      </c>
-      <c r="P3" s="14" t="s">
+      <c r="O3" s="13">
+        <v>0</v>
+      </c>
+      <c r="P3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="U3" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="V3" s="14">
-        <v>0</v>
-      </c>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="14" t="s">
+      <c r="V3" s="13">
+        <v>0</v>
+      </c>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI3" s="18" t="s">
+      <c r="AI3" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AJ3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK3" s="14">
+      <c r="AK3" s="13">
         <v>200</v>
       </c>
-      <c r="AL3" s="14" t="s">
+      <c r="AL3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM3" s="14" t="s">
+      <c r="AM3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN3" s="14">
+      <c r="AN3" s="13">
         <f>G3</f>
         <v>401</v>
       </c>
     </row>
     <row r="4" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <f>G3+1</f>
         <v>402</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="O4" s="14">
-        <v>0</v>
-      </c>
-      <c r="P4" s="14" t="s">
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14">
-        <v>0</v>
-      </c>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
-      <c r="AH4" s="14" t="s">
+      <c r="U4" s="13"/>
+      <c r="V4" s="13">
+        <v>0</v>
+      </c>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI4" s="18" t="s">
+      <c r="AI4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ4" s="12" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK4" s="14">
+      <c r="AK4" s="13">
         <v>200</v>
       </c>
-      <c r="AL4" s="14" t="s">
+      <c r="AL4" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM4" s="14" t="s">
+      <c r="AM4" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN4" s="14">
+      <c r="AN4" s="13">
         <f>G4</f>
         <v>402</v>
       </c>
     </row>
     <row r="5" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <f>G4+1</f>
         <v>403</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="O5" s="14">
-        <v>0</v>
-      </c>
-      <c r="P5" s="14" t="s">
+      <c r="O5" s="13">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14">
-        <v>0</v>
-      </c>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="14" t="s">
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13">
+        <v>0</v>
+      </c>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI5" s="18" t="s">
+      <c r="AI5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ5" s="12" t="s">
+      <c r="AJ5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK5" s="14">
+      <c r="AK5" s="13">
         <v>200</v>
       </c>
-      <c r="AL5" s="14" t="s">
+      <c r="AL5" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM5" s="14" t="s">
+      <c r="AM5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN5" s="14">
+      <c r="AN5" s="13">
         <f>G5</f>
         <v>403</v>
       </c>
     </row>
     <row r="6" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f>G5+1</f>
         <v>404</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="O6" s="14">
-        <v>0</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="O6" s="13">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="S6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14">
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13">
         <v>378</v>
       </c>
-      <c r="W6" s="14">
+      <c r="W6" s="13">
         <v>1600000</v>
       </c>
-      <c r="X6" s="14">
+      <c r="X6" s="13">
         <v>400000</v>
       </c>
-      <c r="Y6" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="18" t="s">
+      <c r="Y6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AC6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="18" t="s">
+      <c r="AC6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AF6" s="18" t="s">
+      <c r="AF6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AG6" s="18" t="s">
+      <c r="AG6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AH6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AI6" s="18" t="s">
+      <c r="AI6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AJ6" s="12" t="s">
+      <c r="AJ6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AK6" s="14">
+      <c r="AK6" s="13">
         <v>200</v>
       </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AL6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AM6" s="14" t="s">
+      <c r="AM6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AN6" s="14">
+      <c r="AN6" s="13">
         <f>G6</f>
         <v>404</v>
       </c>
@@ -4536,7 +4527,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="4" outlineLevelCol="7"/>
@@ -4695,13 +4686,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="19.4285714285714" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
@@ -4796,133 +4787,361 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="20" t="s">
         <v>141</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:13">
-      <c r="A3" s="4" t="s">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="19.4285714285714" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.8571428571429" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+      <c r="A2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:13">
-      <c r="A4" s="4" t="s">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="19.4285714285714" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.8571428571429" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+      <c r="A2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" customHeight="1" spans="1:13">
-      <c r="A5" s="4" t="s">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="19.4285714285714" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.8571428571429" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
+      <c r="A2" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update flow voucher go - course infomation
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CheckIn.xlsx
+++ b/src/main/resources/input_excel_file/booking/CheckIn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Check_In_Bag_Player1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="241">
   <si>
     <t>tc_id</t>
   </si>
@@ -311,6 +311,21 @@
     <t>VST_CI_REMOVE_VC_015</t>
   </si>
   <si>
+    <t>Apply voucher trả trước: Green + Caddie + 1/2 xe + Package</t>
+  </si>
+  <si>
+    <t>VST_CI_006</t>
+  </si>
+  <si>
+    <t>VST_CI_REMOVE_VC_016</t>
+  </si>
+  <si>
+    <t>VST_CI_REMOVE_VC_017</t>
+  </si>
+  <si>
+    <t>VST_CI_REMOVE_VC_018</t>
+  </si>
+  <si>
     <t>CI_PLAYER1_002</t>
   </si>
   <si>
@@ -492,6 +507,33 @@
   </si>
   <si>
     <t>VST_CI_VC_CD4FEE_007</t>
+  </si>
+  <si>
+    <t>VST_CI_VC_TT4FEE_001</t>
+  </si>
+  <si>
+    <t>VST_Kiểm tra check in bag khi nhập voucher trả trước: Green + Caddie + 1/2 xe + Package</t>
+  </si>
+  <si>
+    <t>TT4FEE11</t>
+  </si>
+  <si>
+    <t>VST_CI_VC_TT4FEE_002</t>
+  </si>
+  <si>
+    <t>VST_CI_VC_TT4FEE_003</t>
+  </si>
+  <si>
+    <t>VST_CI_VC_TT4FEE_004</t>
+  </si>
+  <si>
+    <t>VST_CI_VC_TT4FEE_005</t>
+  </si>
+  <si>
+    <t>VST_CI_VC_TT4FEE_006</t>
+  </si>
+  <si>
+    <t>VST_CI_VC_TT4FEE_007</t>
   </si>
   <si>
     <t>CI_VC_GREEN_003</t>
@@ -917,7 +959,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -945,12 +987,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1356,7 +1392,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1380,16 +1416,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1398,89 +1434,89 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1580,14 +1616,11 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2125,10 +2158,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP31"/>
+  <dimension ref="A1:AP36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="$A4:$XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -2297,13 +2332,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" s="33" customFormat="1" ht="26" customHeight="1" spans="1:42">
+    <row r="2" s="10" customFormat="1" ht="26" customHeight="1" spans="1:42">
       <c r="A2" s="20"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -4589,11 +4624,13 @@
     </row>
     <row r="27" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="B27" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="26"/>
       <c r="G27" s="4"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -4633,10 +4670,10 @@
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A28" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>45</v>
@@ -4657,7 +4694,7 @@
         <v>50</v>
       </c>
       <c r="I28" s="7">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>51</v>
@@ -4695,12 +4732,8 @@
       <c r="U28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="V28" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="W28" s="7" t="s">
-        <v>94</v>
-      </c>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
       <c r="X28" s="7">
         <v>0</v>
       </c>
@@ -4734,16 +4767,16 @@
         <v>65</v>
       </c>
       <c r="AP28" s="7">
-        <f>I28</f>
-        <v>104</v>
+        <f t="shared" ref="AP28:AP31" si="4">I28</f>
+        <v>120</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A29" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>45</v>
@@ -4764,7 +4797,7 @@
         <v>50</v>
       </c>
       <c r="I29" s="7">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>51</v>
@@ -4802,9 +4835,7 @@
       <c r="U29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="V29" s="7" t="s">
-        <v>93</v>
-      </c>
+      <c r="V29" s="7"/>
       <c r="W29" s="7"/>
       <c r="X29" s="7">
         <v>0</v>
@@ -4824,7 +4855,7 @@
         <v>61</v>
       </c>
       <c r="AK29" s="19" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AL29" s="5" t="s">
         <v>63</v>
@@ -4839,16 +4870,16 @@
         <v>65</v>
       </c>
       <c r="AP29" s="7">
-        <f>I29</f>
-        <v>105</v>
+        <f t="shared" si="4"/>
+        <v>121</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A30" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>45</v>
@@ -4869,7 +4900,7 @@
         <v>50</v>
       </c>
       <c r="I30" s="7">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>51</v>
@@ -4927,7 +4958,7 @@
         <v>61</v>
       </c>
       <c r="AK30" s="19" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AL30" s="5" t="s">
         <v>63</v>
@@ -4942,22 +4973,22 @@
         <v>65</v>
       </c>
       <c r="AP30" s="7">
-        <f>I30</f>
-        <v>106</v>
+        <f t="shared" si="4"/>
+        <v>122</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="1:42">
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A31" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>47</v>
@@ -4972,7 +5003,7 @@
         <v>50</v>
       </c>
       <c r="I31" s="7">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>51</v>
@@ -5013,46 +5044,24 @@
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7">
-        <v>378</v>
-      </c>
-      <c r="Y31" s="7">
-        <v>1600000</v>
-      </c>
-      <c r="Z31" s="7">
-        <v>400000</v>
-      </c>
-      <c r="AA31" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD31" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE31" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF31" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG31" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH31" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI31" s="19" t="s">
-        <v>62</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="19"/>
+      <c r="AH31" s="19"/>
+      <c r="AI31" s="19"/>
       <c r="AJ31" s="7" t="s">
         <v>61</v>
       </c>
       <c r="AK31" s="19" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AL31" s="5" t="s">
         <v>63</v>
@@ -5067,17 +5076,502 @@
         <v>65</v>
       </c>
       <c r="AP31" s="7">
-        <f>I31</f>
+        <f t="shared" si="4"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:42">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="7"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="19"/>
+      <c r="AI32" s="19"/>
+      <c r="AJ32" s="7"/>
+      <c r="AK32" s="19"/>
+      <c r="AL32" s="5"/>
+      <c r="AM32" s="7"/>
+      <c r="AN32" s="13"/>
+      <c r="AO32" s="7"/>
+      <c r="AP32" s="7"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:42">
+      <c r="A33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="7">
+        <v>104</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>0</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="X33" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="19"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="19"/>
+      <c r="AH33" s="19"/>
+      <c r="AI33" s="19"/>
+      <c r="AJ33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK33" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM33" s="7">
+        <v>200</v>
+      </c>
+      <c r="AN33" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO33" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP33" s="7">
+        <f>I33</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="1" customHeight="1" spans="1:42">
+      <c r="A34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="7">
+        <v>105</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>0</v>
+      </c>
+      <c r="R34" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V34" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="19"/>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="19"/>
+      <c r="AH34" s="19"/>
+      <c r="AI34" s="19"/>
+      <c r="AJ34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK34" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM34" s="7">
+        <v>200</v>
+      </c>
+      <c r="AN34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP34" s="7">
+        <f>I34</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:42">
+      <c r="A35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="7">
+        <v>106</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>0</v>
+      </c>
+      <c r="R35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="19"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="19"/>
+      <c r="AH35" s="19"/>
+      <c r="AI35" s="19"/>
+      <c r="AJ35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK35" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM35" s="7">
+        <v>200</v>
+      </c>
+      <c r="AN35" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO35" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP35" s="7">
+        <f>I35</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" customHeight="1" spans="1:42">
+      <c r="A36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="7">
+        <v>107</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0</v>
+      </c>
+      <c r="R36" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S36" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7">
+        <v>378</v>
+      </c>
+      <c r="Y36" s="7">
+        <v>1600000</v>
+      </c>
+      <c r="Z36" s="7">
+        <v>400000</v>
+      </c>
+      <c r="AA36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH36" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI36" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ36" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK36" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM36" s="7">
+        <v>200</v>
+      </c>
+      <c r="AN36" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO36" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP36" s="7">
+        <f>I36</f>
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B27:F27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -5127,7 +5621,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -5148,27 +5642,27 @@
         <v>38</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>47</v>
@@ -5177,22 +5671,22 @@
         <v>48</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="36" t="s">
-        <v>219</v>
+      <c r="L2" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -5204,10 +5698,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AQ45"/>
+  <dimension ref="A1:AQ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="T29" workbookViewId="0">
-      <selection activeCell="AE39" sqref="AE39"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AS48" sqref="AS48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -5355,10 +5849,10 @@
         <v>34</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="AK1" s="18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="AL1" s="18" t="s">
         <v>36</v>
@@ -5382,7 +5876,7 @@
     <row r="2" s="10" customFormat="1" ht="27" customHeight="1" spans="1:43">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -5428,16 +5922,16 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>47</v>
@@ -5510,7 +6004,7 @@
         <v>35537</v>
       </c>
       <c r="AK3" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AL3" s="19" t="s">
         <v>68</v>
@@ -5534,16 +6028,16 @@
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A4" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>47</v>
@@ -5617,7 +6111,7 @@
         <v>35537</v>
       </c>
       <c r="AK4" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AL4" s="19" t="s">
         <v>68</v>
@@ -5641,16 +6135,16 @@
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A5" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>47</v>
@@ -5724,7 +6218,7 @@
         <v>35537</v>
       </c>
       <c r="AK5" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AL5" s="19" t="s">
         <v>68</v>
@@ -5748,16 +6242,16 @@
     </row>
     <row r="6" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>47</v>
@@ -5831,7 +6325,7 @@
         <v>35537</v>
       </c>
       <c r="AK6" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AL6" s="19" t="s">
         <v>68</v>
@@ -5855,16 +6349,16 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A7" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>47</v>
@@ -5938,7 +6432,7 @@
         <v>35537</v>
       </c>
       <c r="AK7" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AL7" s="19" t="s">
         <v>68</v>
@@ -5962,16 +6456,16 @@
     </row>
     <row r="8" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A8" s="4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>47</v>
@@ -6045,7 +6539,7 @@
         <v>35537</v>
       </c>
       <c r="AK8" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AL8" s="19" t="s">
         <v>68</v>
@@ -6069,16 +6563,16 @@
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A9" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>47</v>
@@ -6152,7 +6646,7 @@
         <v>35537</v>
       </c>
       <c r="AK9" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AL9" s="19" t="s">
         <v>68</v>
@@ -6177,7 +6671,7 @@
     <row r="10" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A10" s="4"/>
       <c r="B10" s="24" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
@@ -6223,16 +6717,16 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="50" customHeight="1" spans="1:43">
       <c r="A11" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>47</v>
@@ -6305,7 +6799,7 @@
         <v>61351</v>
       </c>
       <c r="AK11" s="32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AL11" s="19" t="s">
         <v>68</v>
@@ -6329,16 +6823,16 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="50" customHeight="1" spans="1:43">
       <c r="A12" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>47</v>
@@ -6411,7 +6905,7 @@
         <v>61351</v>
       </c>
       <c r="AK12" s="32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AL12" s="19" t="s">
         <v>68</v>
@@ -6435,16 +6929,16 @@
     </row>
     <row r="13" s="1" customFormat="1" ht="50" customHeight="1" spans="1:43">
       <c r="A13" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>47</v>
@@ -6517,7 +7011,7 @@
         <v>61351</v>
       </c>
       <c r="AK13" s="32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AL13" s="19" t="s">
         <v>68</v>
@@ -6541,16 +7035,16 @@
     </row>
     <row r="14" s="1" customFormat="1" ht="50" customHeight="1" spans="1:43">
       <c r="A14" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>47</v>
@@ -6623,7 +7117,7 @@
         <v>61351</v>
       </c>
       <c r="AK14" s="32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AL14" s="19" t="s">
         <v>68</v>
@@ -6647,16 +7141,16 @@
     </row>
     <row r="15" s="1" customFormat="1" ht="50" customHeight="1" spans="1:43">
       <c r="A15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>47</v>
@@ -6729,7 +7223,7 @@
         <v>61351</v>
       </c>
       <c r="AK15" s="32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AL15" s="19" t="s">
         <v>68</v>
@@ -6753,16 +7247,16 @@
     </row>
     <row r="16" s="1" customFormat="1" ht="50" customHeight="1" spans="1:43">
       <c r="A16" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>47</v>
@@ -6835,7 +7329,7 @@
         <v>61351</v>
       </c>
       <c r="AK16" s="32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AL16" s="19" t="s">
         <v>68</v>
@@ -6859,16 +7353,16 @@
     </row>
     <row r="17" s="1" customFormat="1" ht="50" customHeight="1" spans="1:43">
       <c r="A17" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>47</v>
@@ -6941,7 +7435,7 @@
         <v>61351</v>
       </c>
       <c r="AK17" s="32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AL17" s="19" t="s">
         <v>68</v>
@@ -7012,16 +7506,16 @@
     </row>
     <row r="19" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A19" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>47</v>
@@ -7094,7 +7588,7 @@
         <v>35541</v>
       </c>
       <c r="AK19" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AL19" s="19" t="s">
         <v>68</v>
@@ -7118,16 +7612,16 @@
     </row>
     <row r="20" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A20" s="4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>47</v>
@@ -7200,7 +7694,7 @@
         <v>35541</v>
       </c>
       <c r="AK20" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AL20" s="19" t="s">
         <v>68</v>
@@ -7224,16 +7718,16 @@
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A21" s="4" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>47</v>
@@ -7306,7 +7800,7 @@
         <v>35541</v>
       </c>
       <c r="AK21" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AL21" s="19" t="s">
         <v>68</v>
@@ -7330,16 +7824,16 @@
     </row>
     <row r="22" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A22" s="4" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>47</v>
@@ -7412,7 +7906,7 @@
         <v>35541</v>
       </c>
       <c r="AK22" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AL22" s="19" t="s">
         <v>68</v>
@@ -7436,16 +7930,16 @@
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A23" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>47</v>
@@ -7518,7 +8012,7 @@
         <v>35541</v>
       </c>
       <c r="AK23" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AL23" s="19" t="s">
         <v>68</v>
@@ -7542,16 +8036,16 @@
     </row>
     <row r="24" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A24" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>47</v>
@@ -7624,7 +8118,7 @@
         <v>35541</v>
       </c>
       <c r="AK24" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AL24" s="19" t="s">
         <v>68</v>
@@ -7648,16 +8142,16 @@
     </row>
     <row r="25" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A25" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>47</v>
@@ -7730,7 +8224,7 @@
         <v>35541</v>
       </c>
       <c r="AK25" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AL25" s="19" t="s">
         <v>68</v>
@@ -7801,16 +8295,16 @@
     </row>
     <row r="27" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A27" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>47</v>
@@ -7883,7 +8377,7 @@
         <v>35540</v>
       </c>
       <c r="AK27" s="32" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AL27" s="19" t="s">
         <v>68</v>
@@ -7907,16 +8401,16 @@
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A28" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>47</v>
@@ -7989,7 +8483,7 @@
         <v>35540</v>
       </c>
       <c r="AK28" s="32" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AL28" s="19" t="s">
         <v>68</v>
@@ -8013,16 +8507,16 @@
     </row>
     <row r="29" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A29" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>47</v>
@@ -8095,7 +8589,7 @@
         <v>35540</v>
       </c>
       <c r="AK29" s="32" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AL29" s="19" t="s">
         <v>68</v>
@@ -8119,16 +8613,16 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A30" s="4" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>47</v>
@@ -8201,7 +8695,7 @@
         <v>35540</v>
       </c>
       <c r="AK30" s="32" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AL30" s="19" t="s">
         <v>68</v>
@@ -8225,16 +8719,16 @@
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A31" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>47</v>
@@ -8307,7 +8801,7 @@
         <v>35540</v>
       </c>
       <c r="AK31" s="32" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AL31" s="19" t="s">
         <v>68</v>
@@ -8331,16 +8825,16 @@
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A32" s="4" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>47</v>
@@ -8413,7 +8907,7 @@
         <v>35540</v>
       </c>
       <c r="AK32" s="32" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AL32" s="19" t="s">
         <v>68</v>
@@ -8437,16 +8931,16 @@
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A33" s="4" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>47</v>
@@ -8519,7 +9013,7 @@
         <v>35540</v>
       </c>
       <c r="AK33" s="32" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="AL33" s="19" t="s">
         <v>68</v>
@@ -8590,16 +9084,16 @@
     </row>
     <row r="35" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A35" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>47</v>
@@ -8672,7 +9166,7 @@
         <v>61353</v>
       </c>
       <c r="AK35" s="32" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="AL35" s="19" t="s">
         <v>68</v>
@@ -8696,16 +9190,16 @@
     </row>
     <row r="36" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A36" s="4" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>47</v>
@@ -8778,7 +9272,7 @@
         <v>61353</v>
       </c>
       <c r="AK36" s="32" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="AL36" s="19" t="s">
         <v>68</v>
@@ -8802,16 +9296,16 @@
     </row>
     <row r="37" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A37" s="4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>47</v>
@@ -8884,7 +9378,7 @@
         <v>61353</v>
       </c>
       <c r="AK37" s="32" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="AL37" s="19" t="s">
         <v>68</v>
@@ -8908,16 +9402,16 @@
     </row>
     <row r="38" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A38" s="4" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>47</v>
@@ -8990,7 +9484,7 @@
         <v>61353</v>
       </c>
       <c r="AK38" s="32" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="AL38" s="19" t="s">
         <v>68</v>
@@ -9014,16 +9508,16 @@
     </row>
     <row r="39" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A39" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>47</v>
@@ -9096,7 +9590,7 @@
         <v>61353</v>
       </c>
       <c r="AK39" s="32" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="AL39" s="19" t="s">
         <v>68</v>
@@ -9120,16 +9614,16 @@
     </row>
     <row r="40" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A40" s="4" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>47</v>
@@ -9202,7 +9696,7 @@
         <v>61353</v>
       </c>
       <c r="AK40" s="32" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="AL40" s="19" t="s">
         <v>68</v>
@@ -9226,16 +9720,16 @@
     </row>
     <row r="41" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A41" s="4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>47</v>
@@ -9308,7 +9802,7 @@
         <v>61353</v>
       </c>
       <c r="AK41" s="32" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="AL41" s="19" t="s">
         <v>68</v>
@@ -9332,11 +9826,13 @@
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:43">
       <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
+      <c r="B42" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="4"/>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
@@ -9375,18 +9871,18 @@
       <c r="AP42" s="7"/>
       <c r="AQ42" s="7"/>
     </row>
-    <row r="43" s="1" customFormat="1" customHeight="1" spans="1:43">
+    <row r="43" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A43" s="4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>47</v>
@@ -9401,8 +9897,7 @@
         <v>50</v>
       </c>
       <c r="I43" s="7">
-        <f>I9+1</f>
-        <v>1007</v>
+        <v>1035</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>51</v>
@@ -9440,9 +9935,7 @@
       <c r="U43" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="V43" s="7" t="s">
-        <v>93</v>
-      </c>
+      <c r="V43" s="7"/>
       <c r="W43" s="7"/>
       <c r="X43" s="7">
         <v>0</v>
@@ -9458,10 +9951,14 @@
       <c r="AG43" s="19"/>
       <c r="AH43" s="19"/>
       <c r="AI43" s="19"/>
-      <c r="AJ43" s="7"/>
-      <c r="AK43" s="19"/>
+      <c r="AJ43" s="33">
+        <v>61357</v>
+      </c>
+      <c r="AK43" s="34" t="s">
+        <v>159</v>
+      </c>
       <c r="AL43" s="19" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AM43" s="5" t="s">
         <v>63</v>
@@ -9476,22 +9973,22 @@
         <v>65</v>
       </c>
       <c r="AQ43" s="7">
-        <f>I43</f>
-        <v>1007</v>
+        <f t="shared" ref="AQ43:AQ49" si="6">I43</f>
+        <v>1035</v>
       </c>
     </row>
-    <row r="44" s="1" customFormat="1" customHeight="1" spans="1:43">
+    <row r="44" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A44" s="4" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>47</v>
@@ -9506,8 +10003,7 @@
         <v>50</v>
       </c>
       <c r="I44" s="7">
-        <f>I43+1</f>
-        <v>1008</v>
+        <v>1036</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>51</v>
@@ -9561,10 +10057,14 @@
       <c r="AG44" s="19"/>
       <c r="AH44" s="19"/>
       <c r="AI44" s="19"/>
-      <c r="AJ44" s="7"/>
-      <c r="AK44" s="19"/>
+      <c r="AJ44" s="33">
+        <v>61357</v>
+      </c>
+      <c r="AK44" s="34" t="s">
+        <v>159</v>
+      </c>
       <c r="AL44" s="19" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AM44" s="5" t="s">
         <v>63</v>
@@ -9579,22 +10079,22 @@
         <v>65</v>
       </c>
       <c r="AQ44" s="7">
-        <f>I44</f>
-        <v>1008</v>
+        <f t="shared" si="6"/>
+        <v>1036</v>
       </c>
     </row>
-    <row r="45" customHeight="1" spans="1:43">
+    <row r="45" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
       <c r="A45" s="4" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>47</v>
@@ -9609,8 +10109,7 @@
         <v>50</v>
       </c>
       <c r="I45" s="7">
-        <f>I44+1</f>
-        <v>1009</v>
+        <v>1037</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>51</v>
@@ -9651,45 +10150,27 @@
       <c r="V45" s="7"/>
       <c r="W45" s="7"/>
       <c r="X45" s="7">
-        <v>378</v>
-      </c>
-      <c r="Y45" s="7">
-        <v>1600000</v>
-      </c>
-      <c r="Z45" s="7">
-        <v>400000</v>
-      </c>
-      <c r="AA45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD45" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7"/>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
+      <c r="AC45" s="7"/>
+      <c r="AD45" s="19"/>
+      <c r="AE45" s="7"/>
+      <c r="AF45" s="7"/>
+      <c r="AG45" s="19"/>
+      <c r="AH45" s="19"/>
+      <c r="AI45" s="19"/>
+      <c r="AJ45" s="33">
+        <v>61357</v>
+      </c>
+      <c r="AK45" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL45" s="19" t="s">
         <v>68</v>
-      </c>
-      <c r="AE45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG45" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH45" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI45" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ45" s="7"/>
-      <c r="AK45" s="19"/>
-      <c r="AL45" s="19" t="s">
-        <v>62</v>
       </c>
       <c r="AM45" s="5" t="s">
         <v>63</v>
@@ -9704,17 +10185,820 @@
         <v>65</v>
       </c>
       <c r="AQ45" s="7">
-        <f>I45</f>
+        <f t="shared" si="6"/>
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="46" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
+      <c r="A46" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I46" s="7">
+        <v>1038</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q46" s="7">
+        <v>0</v>
+      </c>
+      <c r="R46" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S46" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="7"/>
+      <c r="AB46" s="7"/>
+      <c r="AC46" s="7"/>
+      <c r="AD46" s="19"/>
+      <c r="AE46" s="7"/>
+      <c r="AF46" s="7"/>
+      <c r="AG46" s="19"/>
+      <c r="AH46" s="19"/>
+      <c r="AI46" s="19"/>
+      <c r="AJ46" s="33">
+        <v>61357</v>
+      </c>
+      <c r="AK46" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL46" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN46" s="7">
+        <v>200</v>
+      </c>
+      <c r="AO46" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP46" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ46" s="7">
+        <f t="shared" si="6"/>
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="47" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
+      <c r="A47" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" s="7">
+        <v>1039</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q47" s="7">
+        <v>0</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T47" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7"/>
+      <c r="AC47" s="7"/>
+      <c r="AD47" s="19"/>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
+      <c r="AG47" s="19"/>
+      <c r="AH47" s="19"/>
+      <c r="AI47" s="19"/>
+      <c r="AJ47" s="33">
+        <v>61357</v>
+      </c>
+      <c r="AK47" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL47" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM47" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN47" s="7">
+        <v>200</v>
+      </c>
+      <c r="AO47" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP47" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ47" s="7">
+        <f t="shared" si="6"/>
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
+      <c r="A48" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48" s="7">
+        <v>1040</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q48" s="7">
+        <v>0</v>
+      </c>
+      <c r="R48" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S48" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T48" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U48" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="7"/>
+      <c r="AB48" s="7"/>
+      <c r="AC48" s="7"/>
+      <c r="AD48" s="19"/>
+      <c r="AE48" s="7"/>
+      <c r="AF48" s="7"/>
+      <c r="AG48" s="19"/>
+      <c r="AH48" s="19"/>
+      <c r="AI48" s="19"/>
+      <c r="AJ48" s="33">
+        <v>61357</v>
+      </c>
+      <c r="AK48" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL48" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM48" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN48" s="7">
+        <v>200</v>
+      </c>
+      <c r="AO48" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP48" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ48" s="7">
+        <f t="shared" si="6"/>
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="49" s="1" customFormat="1" ht="56" customHeight="1" spans="1:43">
+      <c r="A49" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I49" s="7">
+        <v>1041</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q49" s="7">
+        <v>0</v>
+      </c>
+      <c r="R49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T49" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V49" s="7"/>
+      <c r="W49" s="7"/>
+      <c r="X49" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7"/>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7"/>
+      <c r="AC49" s="7"/>
+      <c r="AD49" s="19"/>
+      <c r="AE49" s="7"/>
+      <c r="AF49" s="7"/>
+      <c r="AG49" s="19"/>
+      <c r="AH49" s="19"/>
+      <c r="AI49" s="19"/>
+      <c r="AJ49" s="33">
+        <v>61357</v>
+      </c>
+      <c r="AK49" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL49" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN49" s="7">
+        <v>200</v>
+      </c>
+      <c r="AO49" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP49" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ49" s="7">
+        <f t="shared" si="6"/>
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="1" customHeight="1" spans="1:43">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="7"/>
+      <c r="AB50" s="7"/>
+      <c r="AC50" s="7"/>
+      <c r="AD50" s="19"/>
+      <c r="AE50" s="7"/>
+      <c r="AF50" s="7"/>
+      <c r="AG50" s="19"/>
+      <c r="AH50" s="19"/>
+      <c r="AI50" s="19"/>
+      <c r="AJ50" s="7"/>
+      <c r="AK50" s="30"/>
+      <c r="AL50" s="19"/>
+      <c r="AM50" s="5"/>
+      <c r="AN50" s="7"/>
+      <c r="AO50" s="13"/>
+      <c r="AP50" s="7"/>
+      <c r="AQ50" s="7"/>
+    </row>
+    <row r="51" s="1" customFormat="1" customHeight="1" spans="1:43">
+      <c r="A51" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I51" s="7">
+        <f>I9+1</f>
+        <v>1007</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N51" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P51" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q51" s="7">
+        <v>0</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T51" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U51" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="W51" s="7"/>
+      <c r="X51" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="7"/>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7"/>
+      <c r="AC51" s="7"/>
+      <c r="AD51" s="19"/>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="19"/>
+      <c r="AH51" s="19"/>
+      <c r="AI51" s="19"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="19"/>
+      <c r="AL51" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN51" s="7">
+        <v>200</v>
+      </c>
+      <c r="AO51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP51" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ51" s="7">
+        <f>I51</f>
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="52" s="1" customFormat="1" customHeight="1" spans="1:43">
+      <c r="A52" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I52" s="7">
+        <f>I51+1</f>
+        <v>1008</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P52" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q52" s="7">
+        <v>0</v>
+      </c>
+      <c r="R52" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T52" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U52" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V52" s="7"/>
+      <c r="W52" s="7"/>
+      <c r="X52" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="7"/>
+      <c r="Z52" s="7"/>
+      <c r="AA52" s="7"/>
+      <c r="AB52" s="7"/>
+      <c r="AC52" s="7"/>
+      <c r="AD52" s="19"/>
+      <c r="AE52" s="7"/>
+      <c r="AF52" s="7"/>
+      <c r="AG52" s="19"/>
+      <c r="AH52" s="19"/>
+      <c r="AI52" s="19"/>
+      <c r="AJ52" s="7"/>
+      <c r="AK52" s="19"/>
+      <c r="AL52" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN52" s="7">
+        <v>200</v>
+      </c>
+      <c r="AO52" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP52" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ52" s="7">
+        <f>I52</f>
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="53" customHeight="1" spans="1:43">
+      <c r="A53" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I53" s="7">
+        <f>I52+1</f>
+        <v>1009</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O53" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P53" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q53" s="7">
+        <v>0</v>
+      </c>
+      <c r="R53" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T53" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U53" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="7">
+        <v>378</v>
+      </c>
+      <c r="Y53" s="7">
+        <v>1600000</v>
+      </c>
+      <c r="Z53" s="7">
+        <v>400000</v>
+      </c>
+      <c r="AA53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="19"/>
+      <c r="AL53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM53" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN53" s="7">
+        <v>200</v>
+      </c>
+      <c r="AO53" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP53" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ53" s="7">
+        <f>I53</f>
         <v>1009</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B42:F42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -9898,7 +11182,7 @@
     </row>
     <row r="2" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A2" s="5" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>44</v>
@@ -9925,25 +11209,25 @@
         <v>200</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="Q2" s="13">
         <v>0</v>
@@ -10001,10 +11285,10 @@
     </row>
     <row r="3" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A3" s="5" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>45</v>
@@ -10029,25 +11313,25 @@
         <v>201</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="Q3" s="13">
         <v>0</v>
@@ -10065,10 +11349,10 @@
         <v>49</v>
       </c>
       <c r="V3" s="13" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="W3" s="13" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="X3" s="13">
         <v>0</v>
@@ -10109,10 +11393,10 @@
     </row>
     <row r="4" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A4" s="5" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>45</v>
@@ -10137,25 +11421,25 @@
         <v>202</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="Q4" s="13">
         <v>0</v>
@@ -10173,7 +11457,7 @@
         <v>49</v>
       </c>
       <c r="V4" s="13" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="W4" s="13"/>
       <c r="X4" s="13">
@@ -10215,10 +11499,10 @@
     </row>
     <row r="5" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A5" s="5" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>45</v>
@@ -10243,25 +11527,25 @@
         <v>203</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="Q5" s="13">
         <v>0</v>
@@ -10319,16 +11603,16 @@
     </row>
     <row r="6" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A6" s="5" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>47</v>
@@ -10347,25 +11631,25 @@
         <v>204</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="Q6" s="13">
         <v>0</v>
@@ -10628,7 +11912,7 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A2" s="4" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>44</v>
@@ -10655,25 +11939,25 @@
         <v>300</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="Q2" s="7">
         <v>0</v>
@@ -10731,10 +12015,10 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A3" s="4" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>45</v>
@@ -10759,25 +12043,25 @@
         <v>301</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="Q3" s="7">
         <v>0</v>
@@ -10795,10 +12079,10 @@
         <v>49</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="X3" s="7">
         <v>0</v>
@@ -10839,10 +12123,10 @@
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A4" s="4" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>45</v>
@@ -10867,25 +12151,25 @@
         <v>302</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="Q4" s="7">
         <v>0</v>
@@ -10903,7 +12187,7 @@
         <v>49</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="W4" s="7"/>
       <c r="X4" s="7">
@@ -10945,10 +12229,10 @@
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:42">
       <c r="A5" s="4" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>45</v>
@@ -10973,25 +12257,25 @@
         <v>303</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="Q5" s="7">
         <v>0</v>
@@ -11049,16 +12333,16 @@
     </row>
     <row r="6" customHeight="1" spans="1:42">
       <c r="A6" s="4" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>47</v>
@@ -11077,25 +12361,25 @@
         <v>304</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
@@ -11356,7 +12640,7 @@
     </row>
     <row r="2" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A2" s="5" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>44</v>
@@ -11383,25 +12667,25 @@
         <v>400</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="Q2" s="13">
         <v>0</v>
@@ -11459,10 +12743,10 @@
     </row>
     <row r="3" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A3" s="5" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>45</v>
@@ -11487,25 +12771,25 @@
         <v>401</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="Q3" s="13">
         <v>0</v>
@@ -11523,10 +12807,10 @@
         <v>49</v>
       </c>
       <c r="V3" s="13" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="W3" s="13" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="X3" s="13">
         <v>0</v>
@@ -11567,10 +12851,10 @@
     </row>
     <row r="4" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A4" s="5" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>45</v>
@@ -11595,25 +12879,25 @@
         <v>402</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="Q4" s="13">
         <v>0</v>
@@ -11631,7 +12915,7 @@
         <v>49</v>
       </c>
       <c r="V4" s="13" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="W4" s="13"/>
       <c r="X4" s="13">
@@ -11673,10 +12957,10 @@
     </row>
     <row r="5" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A5" s="5" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>45</v>
@@ -11701,25 +12985,25 @@
         <v>403</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="Q5" s="13">
         <v>0</v>
@@ -11777,16 +13061,16 @@
     </row>
     <row r="6" s="10" customFormat="1" customHeight="1" spans="1:42">
       <c r="A6" s="5" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>47</v>
@@ -11805,25 +13089,25 @@
         <v>404</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="Q6" s="13">
         <v>0</v>
@@ -11961,25 +13245,25 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="H2" s="7">
         <v>200</v>
@@ -11987,25 +13271,25 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="H3" s="7">
         <v>200</v>
@@ -12013,25 +13297,25 @@
     </row>
     <row r="4" customHeight="1" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="H4" s="7">
         <v>200</v>
@@ -12039,25 +13323,25 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="H5" s="7">
         <v>200</v>
@@ -12112,7 +13396,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -12133,27 +13417,27 @@
         <v>38</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>47</v>
@@ -12165,19 +13449,19 @@
         <v>50</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="36" t="s">
-        <v>219</v>
+      <c r="L2" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -12229,7 +13513,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -12250,27 +13534,27 @@
         <v>38</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>47</v>
@@ -12279,22 +13563,22 @@
         <v>48</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="36" t="s">
-        <v>219</v>
+      <c r="L2" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -12346,7 +13630,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -12367,27 +13651,27 @@
         <v>38</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>47</v>
@@ -12396,22 +13680,22 @@
         <v>48</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="36" t="s">
-        <v>219</v>
+      <c r="L2" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run create flighht round 2
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CheckIn.xlsx
+++ b/src/main/resources/input_excel_file/booking/CheckIn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Check_In_Bag_Player1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
     <t>check_in_bag_1_voucher_request.json</t>
   </si>
   <si>
-    <t>GR0001</t>
+    <t>GREEN41</t>
   </si>
   <si>
     <t>VST_CI_VC_GREEN_002</t>
@@ -1208,7 +1208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1230,12 +1230,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1660,7 +1654,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1684,16 +1678,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1702,89 +1696,89 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1848,16 +1842,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1881,16 +1875,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1902,22 +1896,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -2458,10 +2449,10 @@
   <sheetPr/>
   <dimension ref="A1:AZ68"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44:F46"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -9376,7 +9367,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="44" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">
@@ -9394,10 +9385,10 @@
   <sheetPr/>
   <dimension ref="A1:AZ103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E107" sqref="E107"/>
+      <selection pane="bottomLeft" activeCell="AS10" sqref="AS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -9752,10 +9743,10 @@
       <c r="AG4" s="19"/>
       <c r="AH4" s="19"/>
       <c r="AI4" s="19"/>
-      <c r="AJ4" s="5">
-        <v>35537</v>
-      </c>
-      <c r="AK4" s="39" t="s">
+      <c r="AJ4" s="39">
+        <v>61373</v>
+      </c>
+      <c r="AK4" s="40" t="s">
         <v>141</v>
       </c>
       <c r="AL4" s="19" t="s">
@@ -9859,10 +9850,10 @@
       <c r="AG5" s="19"/>
       <c r="AH5" s="19"/>
       <c r="AI5" s="19"/>
-      <c r="AJ5" s="5">
-        <v>35537</v>
-      </c>
-      <c r="AK5" s="39" t="s">
+      <c r="AJ5" s="39">
+        <v>61373</v>
+      </c>
+      <c r="AK5" s="40" t="s">
         <v>141</v>
       </c>
       <c r="AL5" s="19" t="s">
@@ -9966,10 +9957,10 @@
       <c r="AG6" s="19"/>
       <c r="AH6" s="19"/>
       <c r="AI6" s="19"/>
-      <c r="AJ6" s="5">
-        <v>35537</v>
-      </c>
-      <c r="AK6" s="39" t="s">
+      <c r="AJ6" s="39">
+        <v>61373</v>
+      </c>
+      <c r="AK6" s="40" t="s">
         <v>141</v>
       </c>
       <c r="AL6" s="19" t="s">
@@ -10073,10 +10064,10 @@
       <c r="AG7" s="19"/>
       <c r="AH7" s="19"/>
       <c r="AI7" s="19"/>
-      <c r="AJ7" s="5">
-        <v>35537</v>
-      </c>
-      <c r="AK7" s="39" t="s">
+      <c r="AJ7" s="39">
+        <v>61373</v>
+      </c>
+      <c r="AK7" s="40" t="s">
         <v>141</v>
       </c>
       <c r="AL7" s="19" t="s">
@@ -10180,10 +10171,10 @@
       <c r="AG8" s="19"/>
       <c r="AH8" s="19"/>
       <c r="AI8" s="19"/>
-      <c r="AJ8" s="5">
-        <v>35537</v>
-      </c>
-      <c r="AK8" s="39" t="s">
+      <c r="AJ8" s="39">
+        <v>61373</v>
+      </c>
+      <c r="AK8" s="40" t="s">
         <v>141</v>
       </c>
       <c r="AL8" s="19" t="s">
@@ -10287,10 +10278,10 @@
       <c r="AG9" s="19"/>
       <c r="AH9" s="19"/>
       <c r="AI9" s="19"/>
-      <c r="AJ9" s="5">
-        <v>35537</v>
-      </c>
-      <c r="AK9" s="39" t="s">
+      <c r="AJ9" s="39">
+        <v>61373</v>
+      </c>
+      <c r="AK9" s="40" t="s">
         <v>141</v>
       </c>
       <c r="AL9" s="19" t="s">
@@ -10394,10 +10385,10 @@
       <c r="AG10" s="19"/>
       <c r="AH10" s="19"/>
       <c r="AI10" s="19"/>
-      <c r="AJ10" s="5">
-        <v>35537</v>
-      </c>
-      <c r="AK10" s="39" t="s">
+      <c r="AJ10" s="39">
+        <v>61373</v>
+      </c>
+      <c r="AK10" s="40" t="s">
         <v>141</v>
       </c>
       <c r="AL10" s="19" t="s">
@@ -10459,7 +10450,7 @@
       <c r="AH11" s="19"/>
       <c r="AI11" s="19"/>
       <c r="AJ11" s="7"/>
-      <c r="AK11" s="40"/>
+      <c r="AK11" s="41"/>
       <c r="AL11" s="19"/>
       <c r="AM11" s="5"/>
       <c r="AN11" s="7"/>
@@ -10547,10 +10538,10 @@
       <c r="AG12" s="19"/>
       <c r="AH12" s="19"/>
       <c r="AI12" s="19"/>
-      <c r="AJ12" s="41">
+      <c r="AJ12" s="42">
         <v>61351</v>
       </c>
-      <c r="AK12" s="42" t="s">
+      <c r="AK12" s="43" t="s">
         <v>151</v>
       </c>
       <c r="AL12" s="19" t="s">
@@ -10653,10 +10644,10 @@
       <c r="AG13" s="19"/>
       <c r="AH13" s="19"/>
       <c r="AI13" s="19"/>
-      <c r="AJ13" s="41">
+      <c r="AJ13" s="42">
         <v>61351</v>
       </c>
-      <c r="AK13" s="42" t="s">
+      <c r="AK13" s="43" t="s">
         <v>151</v>
       </c>
       <c r="AL13" s="19" t="s">
@@ -10759,10 +10750,10 @@
       <c r="AG14" s="19"/>
       <c r="AH14" s="19"/>
       <c r="AI14" s="19"/>
-      <c r="AJ14" s="41">
+      <c r="AJ14" s="42">
         <v>61351</v>
       </c>
-      <c r="AK14" s="42" t="s">
+      <c r="AK14" s="43" t="s">
         <v>151</v>
       </c>
       <c r="AL14" s="19" t="s">
@@ -10865,10 +10856,10 @@
       <c r="AG15" s="19"/>
       <c r="AH15" s="19"/>
       <c r="AI15" s="19"/>
-      <c r="AJ15" s="41">
+      <c r="AJ15" s="42">
         <v>61351</v>
       </c>
-      <c r="AK15" s="42" t="s">
+      <c r="AK15" s="43" t="s">
         <v>151</v>
       </c>
       <c r="AL15" s="19" t="s">
@@ -10971,10 +10962,10 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
       <c r="AI16" s="19"/>
-      <c r="AJ16" s="41">
+      <c r="AJ16" s="42">
         <v>61351</v>
       </c>
-      <c r="AK16" s="42" t="s">
+      <c r="AK16" s="43" t="s">
         <v>151</v>
       </c>
       <c r="AL16" s="19" t="s">
@@ -11077,10 +11068,10 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
       <c r="AI17" s="19"/>
-      <c r="AJ17" s="41">
+      <c r="AJ17" s="42">
         <v>61351</v>
       </c>
-      <c r="AK17" s="42" t="s">
+      <c r="AK17" s="43" t="s">
         <v>151</v>
       </c>
       <c r="AL17" s="19" t="s">
@@ -11183,10 +11174,10 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
       <c r="AI18" s="19"/>
-      <c r="AJ18" s="41">
+      <c r="AJ18" s="42">
         <v>61351</v>
       </c>
-      <c r="AK18" s="42" t="s">
+      <c r="AK18" s="43" t="s">
         <v>151</v>
       </c>
       <c r="AL18" s="19" t="s">
@@ -11248,7 +11239,7 @@
       <c r="AH19" s="19"/>
       <c r="AI19" s="19"/>
       <c r="AJ19" s="7"/>
-      <c r="AK19" s="40"/>
+      <c r="AK19" s="41"/>
       <c r="AL19" s="19"/>
       <c r="AM19" s="5"/>
       <c r="AN19" s="7"/>
@@ -11336,10 +11327,10 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
       <c r="AI20" s="19"/>
-      <c r="AJ20" s="41">
+      <c r="AJ20" s="42">
         <v>35541</v>
       </c>
-      <c r="AK20" s="42" t="s">
+      <c r="AK20" s="43" t="s">
         <v>160</v>
       </c>
       <c r="AL20" s="19" t="s">
@@ -11442,10 +11433,10 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
       <c r="AI21" s="19"/>
-      <c r="AJ21" s="41">
+      <c r="AJ21" s="42">
         <v>35541</v>
       </c>
-      <c r="AK21" s="42" t="s">
+      <c r="AK21" s="43" t="s">
         <v>160</v>
       </c>
       <c r="AL21" s="19" t="s">
@@ -11548,10 +11539,10 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
       <c r="AI22" s="19"/>
-      <c r="AJ22" s="41">
+      <c r="AJ22" s="42">
         <v>35541</v>
       </c>
-      <c r="AK22" s="42" t="s">
+      <c r="AK22" s="43" t="s">
         <v>160</v>
       </c>
       <c r="AL22" s="19" t="s">
@@ -11654,10 +11645,10 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
       <c r="AI23" s="19"/>
-      <c r="AJ23" s="41">
+      <c r="AJ23" s="42">
         <v>35541</v>
       </c>
-      <c r="AK23" s="42" t="s">
+      <c r="AK23" s="43" t="s">
         <v>160</v>
       </c>
       <c r="AL23" s="19" t="s">
@@ -11760,10 +11751,10 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
       <c r="AI24" s="19"/>
-      <c r="AJ24" s="41">
+      <c r="AJ24" s="42">
         <v>35541</v>
       </c>
-      <c r="AK24" s="42" t="s">
+      <c r="AK24" s="43" t="s">
         <v>160</v>
       </c>
       <c r="AL24" s="19" t="s">
@@ -11866,10 +11857,10 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
       <c r="AI25" s="19"/>
-      <c r="AJ25" s="41">
+      <c r="AJ25" s="42">
         <v>35541</v>
       </c>
-      <c r="AK25" s="42" t="s">
+      <c r="AK25" s="43" t="s">
         <v>160</v>
       </c>
       <c r="AL25" s="19" t="s">
@@ -11972,10 +11963,10 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
       <c r="AI26" s="19"/>
-      <c r="AJ26" s="41">
+      <c r="AJ26" s="42">
         <v>35541</v>
       </c>
-      <c r="AK26" s="42" t="s">
+      <c r="AK26" s="43" t="s">
         <v>160</v>
       </c>
       <c r="AL26" s="19" t="s">
@@ -12037,7 +12028,7 @@
       <c r="AH27" s="19"/>
       <c r="AI27" s="19"/>
       <c r="AJ27" s="7"/>
-      <c r="AK27" s="40"/>
+      <c r="AK27" s="41"/>
       <c r="AL27" s="19"/>
       <c r="AM27" s="5"/>
       <c r="AN27" s="7"/>
@@ -12125,10 +12116,10 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
       <c r="AI28" s="19"/>
-      <c r="AJ28" s="41">
+      <c r="AJ28" s="42">
         <v>35540</v>
       </c>
-      <c r="AK28" s="42" t="s">
+      <c r="AK28" s="43" t="s">
         <v>169</v>
       </c>
       <c r="AL28" s="19" t="s">
@@ -12231,10 +12222,10 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
       <c r="AI29" s="19"/>
-      <c r="AJ29" s="41">
+      <c r="AJ29" s="42">
         <v>35540</v>
       </c>
-      <c r="AK29" s="42" t="s">
+      <c r="AK29" s="43" t="s">
         <v>169</v>
       </c>
       <c r="AL29" s="19" t="s">
@@ -12337,10 +12328,10 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
       <c r="AI30" s="19"/>
-      <c r="AJ30" s="41">
+      <c r="AJ30" s="42">
         <v>35540</v>
       </c>
-      <c r="AK30" s="42" t="s">
+      <c r="AK30" s="43" t="s">
         <v>169</v>
       </c>
       <c r="AL30" s="19" t="s">
@@ -12443,10 +12434,10 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
       <c r="AI31" s="19"/>
-      <c r="AJ31" s="41">
+      <c r="AJ31" s="42">
         <v>35540</v>
       </c>
-      <c r="AK31" s="42" t="s">
+      <c r="AK31" s="43" t="s">
         <v>169</v>
       </c>
       <c r="AL31" s="19" t="s">
@@ -12549,10 +12540,10 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
       <c r="AI32" s="19"/>
-      <c r="AJ32" s="41">
+      <c r="AJ32" s="42">
         <v>35540</v>
       </c>
-      <c r="AK32" s="42" t="s">
+      <c r="AK32" s="43" t="s">
         <v>169</v>
       </c>
       <c r="AL32" s="19" t="s">
@@ -12655,10 +12646,10 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
       <c r="AI33" s="19"/>
-      <c r="AJ33" s="41">
+      <c r="AJ33" s="42">
         <v>35540</v>
       </c>
-      <c r="AK33" s="42" t="s">
+      <c r="AK33" s="43" t="s">
         <v>169</v>
       </c>
       <c r="AL33" s="19" t="s">
@@ -12761,10 +12752,10 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
       <c r="AI34" s="19"/>
-      <c r="AJ34" s="41">
+      <c r="AJ34" s="42">
         <v>35540</v>
       </c>
-      <c r="AK34" s="42" t="s">
+      <c r="AK34" s="43" t="s">
         <v>169</v>
       </c>
       <c r="AL34" s="19" t="s">
@@ -12826,7 +12817,7 @@
       <c r="AH35" s="19"/>
       <c r="AI35" s="19"/>
       <c r="AJ35" s="7"/>
-      <c r="AK35" s="40"/>
+      <c r="AK35" s="41"/>
       <c r="AL35" s="19"/>
       <c r="AM35" s="5"/>
       <c r="AN35" s="7"/>
@@ -12914,10 +12905,10 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
       <c r="AI36" s="19"/>
-      <c r="AJ36" s="41">
+      <c r="AJ36" s="42">
         <v>61353</v>
       </c>
-      <c r="AK36" s="42" t="s">
+      <c r="AK36" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AL36" s="19" t="s">
@@ -13020,10 +13011,10 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
       <c r="AI37" s="19"/>
-      <c r="AJ37" s="41">
+      <c r="AJ37" s="42">
         <v>61353</v>
       </c>
-      <c r="AK37" s="42" t="s">
+      <c r="AK37" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AL37" s="19" t="s">
@@ -13126,10 +13117,10 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
       <c r="AI38" s="19"/>
-      <c r="AJ38" s="41">
+      <c r="AJ38" s="42">
         <v>61353</v>
       </c>
-      <c r="AK38" s="42" t="s">
+      <c r="AK38" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AL38" s="19" t="s">
@@ -13232,10 +13223,10 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
       <c r="AI39" s="19"/>
-      <c r="AJ39" s="41">
+      <c r="AJ39" s="42">
         <v>61353</v>
       </c>
-      <c r="AK39" s="42" t="s">
+      <c r="AK39" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AL39" s="19" t="s">
@@ -13338,10 +13329,10 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
       <c r="AI40" s="19"/>
-      <c r="AJ40" s="41">
+      <c r="AJ40" s="42">
         <v>61353</v>
       </c>
-      <c r="AK40" s="42" t="s">
+      <c r="AK40" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AL40" s="19" t="s">
@@ -13444,10 +13435,10 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
       <c r="AI41" s="19"/>
-      <c r="AJ41" s="41">
+      <c r="AJ41" s="42">
         <v>61353</v>
       </c>
-      <c r="AK41" s="42" t="s">
+      <c r="AK41" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AL41" s="19" t="s">
@@ -13550,10 +13541,10 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
       <c r="AI42" s="19"/>
-      <c r="AJ42" s="41">
+      <c r="AJ42" s="42">
         <v>61353</v>
       </c>
-      <c r="AK42" s="42" t="s">
+      <c r="AK42" s="43" t="s">
         <v>178</v>
       </c>
       <c r="AL42" s="19" t="s">
@@ -13615,7 +13606,7 @@
       <c r="AH43" s="19"/>
       <c r="AI43" s="19"/>
       <c r="AJ43" s="7"/>
-      <c r="AK43" s="40"/>
+      <c r="AK43" s="41"/>
       <c r="AL43" s="19"/>
       <c r="AM43" s="5"/>
       <c r="AN43" s="7"/>
@@ -13703,10 +13694,10 @@
       <c r="AG44" s="19"/>
       <c r="AH44" s="19"/>
       <c r="AI44" s="19"/>
-      <c r="AJ44" s="41">
+      <c r="AJ44" s="42">
         <v>61357</v>
       </c>
-      <c r="AK44" s="42" t="s">
+      <c r="AK44" s="43" t="s">
         <v>187</v>
       </c>
       <c r="AL44" s="19" t="s">
@@ -13809,10 +13800,10 @@
       <c r="AG45" s="19"/>
       <c r="AH45" s="19"/>
       <c r="AI45" s="19"/>
-      <c r="AJ45" s="41">
+      <c r="AJ45" s="42">
         <v>61357</v>
       </c>
-      <c r="AK45" s="42" t="s">
+      <c r="AK45" s="43" t="s">
         <v>187</v>
       </c>
       <c r="AL45" s="19" t="s">
@@ -13915,10 +13906,10 @@
       <c r="AG46" s="19"/>
       <c r="AH46" s="19"/>
       <c r="AI46" s="19"/>
-      <c r="AJ46" s="41">
+      <c r="AJ46" s="42">
         <v>61357</v>
       </c>
-      <c r="AK46" s="42" t="s">
+      <c r="AK46" s="43" t="s">
         <v>187</v>
       </c>
       <c r="AL46" s="19" t="s">
@@ -14021,10 +14012,10 @@
       <c r="AG47" s="19"/>
       <c r="AH47" s="19"/>
       <c r="AI47" s="19"/>
-      <c r="AJ47" s="41">
+      <c r="AJ47" s="42">
         <v>61357</v>
       </c>
-      <c r="AK47" s="42" t="s">
+      <c r="AK47" s="43" t="s">
         <v>187</v>
       </c>
       <c r="AL47" s="19" t="s">
@@ -14127,10 +14118,10 @@
       <c r="AG48" s="19"/>
       <c r="AH48" s="19"/>
       <c r="AI48" s="19"/>
-      <c r="AJ48" s="41">
+      <c r="AJ48" s="42">
         <v>61357</v>
       </c>
-      <c r="AK48" s="42" t="s">
+      <c r="AK48" s="43" t="s">
         <v>187</v>
       </c>
       <c r="AL48" s="19" t="s">
@@ -14233,10 +14224,10 @@
       <c r="AG49" s="19"/>
       <c r="AH49" s="19"/>
       <c r="AI49" s="19"/>
-      <c r="AJ49" s="41">
+      <c r="AJ49" s="42">
         <v>61357</v>
       </c>
-      <c r="AK49" s="42" t="s">
+      <c r="AK49" s="43" t="s">
         <v>187</v>
       </c>
       <c r="AL49" s="19" t="s">
@@ -14339,10 +14330,10 @@
       <c r="AG50" s="19"/>
       <c r="AH50" s="19"/>
       <c r="AI50" s="19"/>
-      <c r="AJ50" s="41">
+      <c r="AJ50" s="42">
         <v>61357</v>
       </c>
-      <c r="AK50" s="42" t="s">
+      <c r="AK50" s="43" t="s">
         <v>187</v>
       </c>
       <c r="AL50" s="19" t="s">
@@ -14570,10 +14561,10 @@
       <c r="AI53" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ53" s="43">
+      <c r="AJ53" s="42">
         <v>61361</v>
       </c>
-      <c r="AK53" s="44" t="s">
+      <c r="AK53" s="43" t="s">
         <v>197</v>
       </c>
       <c r="AL53" s="19" t="s">
@@ -14699,10 +14690,10 @@
       <c r="AI54" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ54" s="43">
+      <c r="AJ54" s="42">
         <v>61361</v>
       </c>
-      <c r="AK54" s="44" t="s">
+      <c r="AK54" s="43" t="s">
         <v>197</v>
       </c>
       <c r="AL54" s="19" t="s">
@@ -14828,10 +14819,10 @@
       <c r="AI55" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ55" s="43">
+      <c r="AJ55" s="42">
         <v>61361</v>
       </c>
-      <c r="AK55" s="44" t="s">
+      <c r="AK55" s="43" t="s">
         <v>197</v>
       </c>
       <c r="AL55" s="19" t="s">
@@ -14957,10 +14948,10 @@
       <c r="AI56" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ56" s="43">
+      <c r="AJ56" s="42">
         <v>61361</v>
       </c>
-      <c r="AK56" s="44" t="s">
+      <c r="AK56" s="43" t="s">
         <v>197</v>
       </c>
       <c r="AL56" s="19" t="s">
@@ -15086,10 +15077,10 @@
       <c r="AI57" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ57" s="43">
+      <c r="AJ57" s="42">
         <v>61361</v>
       </c>
-      <c r="AK57" s="44" t="s">
+      <c r="AK57" s="43" t="s">
         <v>197</v>
       </c>
       <c r="AL57" s="19" t="s">
@@ -15215,10 +15206,10 @@
       <c r="AI58" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ58" s="43">
+      <c r="AJ58" s="42">
         <v>61361</v>
       </c>
-      <c r="AK58" s="44" t="s">
+      <c r="AK58" s="43" t="s">
         <v>197</v>
       </c>
       <c r="AL58" s="19" t="s">
@@ -15344,10 +15335,10 @@
       <c r="AI59" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ59" s="43">
+      <c r="AJ59" s="42">
         <v>61361</v>
       </c>
-      <c r="AK59" s="44" t="s">
+      <c r="AK59" s="43" t="s">
         <v>197</v>
       </c>
       <c r="AL59" s="19" t="s">
@@ -15409,7 +15400,7 @@
       <c r="AH60" s="19"/>
       <c r="AI60" s="19"/>
       <c r="AJ60" s="7"/>
-      <c r="AK60" s="40"/>
+      <c r="AK60" s="41"/>
       <c r="AL60" s="19"/>
       <c r="AM60" s="5"/>
       <c r="AN60" s="7"/>
@@ -15519,10 +15510,10 @@
       <c r="AI61" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ61" s="43">
+      <c r="AJ61" s="42">
         <v>61362</v>
       </c>
-      <c r="AK61" s="44" t="s">
+      <c r="AK61" s="43" t="s">
         <v>206</v>
       </c>
       <c r="AL61" s="19" t="s">
@@ -15647,10 +15638,10 @@
       <c r="AI62" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ62" s="43">
+      <c r="AJ62" s="42">
         <v>61362</v>
       </c>
-      <c r="AK62" s="44" t="s">
+      <c r="AK62" s="43" t="s">
         <v>206</v>
       </c>
       <c r="AL62" s="19" t="s">
@@ -15775,10 +15766,10 @@
       <c r="AI63" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ63" s="43">
+      <c r="AJ63" s="42">
         <v>61362</v>
       </c>
-      <c r="AK63" s="44" t="s">
+      <c r="AK63" s="43" t="s">
         <v>206</v>
       </c>
       <c r="AL63" s="19" t="s">
@@ -15903,10 +15894,10 @@
       <c r="AI64" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ64" s="43">
+      <c r="AJ64" s="42">
         <v>61362</v>
       </c>
-      <c r="AK64" s="44" t="s">
+      <c r="AK64" s="43" t="s">
         <v>206</v>
       </c>
       <c r="AL64" s="19" t="s">
@@ -16031,10 +16022,10 @@
       <c r="AI65" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ65" s="43">
+      <c r="AJ65" s="42">
         <v>61362</v>
       </c>
-      <c r="AK65" s="44" t="s">
+      <c r="AK65" s="43" t="s">
         <v>206</v>
       </c>
       <c r="AL65" s="19" t="s">
@@ -16159,10 +16150,10 @@
       <c r="AI66" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ66" s="43">
+      <c r="AJ66" s="42">
         <v>61362</v>
       </c>
-      <c r="AK66" s="44" t="s">
+      <c r="AK66" s="43" t="s">
         <v>206</v>
       </c>
       <c r="AL66" s="19" t="s">
@@ -16287,10 +16278,10 @@
       <c r="AI67" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ67" s="43">
+      <c r="AJ67" s="42">
         <v>61362</v>
       </c>
-      <c r="AK67" s="44" t="s">
+      <c r="AK67" s="43" t="s">
         <v>206</v>
       </c>
       <c r="AL67" s="19" t="s">
@@ -16352,7 +16343,7 @@
       <c r="AH68" s="19"/>
       <c r="AI68" s="19"/>
       <c r="AJ68" s="7"/>
-      <c r="AK68" s="40"/>
+      <c r="AK68" s="41"/>
       <c r="AL68" s="19"/>
       <c r="AM68" s="5"/>
       <c r="AN68" s="7"/>
@@ -16462,10 +16453,10 @@
       <c r="AI69" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ69" s="43">
+      <c r="AJ69" s="42">
         <v>61363</v>
       </c>
-      <c r="AK69" s="44" t="s">
+      <c r="AK69" s="43" t="s">
         <v>215</v>
       </c>
       <c r="AL69" s="19" t="s">
@@ -16590,10 +16581,10 @@
       <c r="AI70" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ70" s="43">
+      <c r="AJ70" s="42">
         <v>61363</v>
       </c>
-      <c r="AK70" s="44" t="s">
+      <c r="AK70" s="43" t="s">
         <v>215</v>
       </c>
       <c r="AL70" s="19" t="s">
@@ -16718,10 +16709,10 @@
       <c r="AI71" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ71" s="43">
+      <c r="AJ71" s="42">
         <v>61363</v>
       </c>
-      <c r="AK71" s="44" t="s">
+      <c r="AK71" s="43" t="s">
         <v>215</v>
       </c>
       <c r="AL71" s="19" t="s">
@@ -16846,10 +16837,10 @@
       <c r="AI72" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ72" s="43">
+      <c r="AJ72" s="42">
         <v>61363</v>
       </c>
-      <c r="AK72" s="44" t="s">
+      <c r="AK72" s="43" t="s">
         <v>215</v>
       </c>
       <c r="AL72" s="19" t="s">
@@ -16974,10 +16965,10 @@
       <c r="AI73" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ73" s="43">
+      <c r="AJ73" s="42">
         <v>61363</v>
       </c>
-      <c r="AK73" s="44" t="s">
+      <c r="AK73" s="43" t="s">
         <v>215</v>
       </c>
       <c r="AL73" s="19" t="s">
@@ -17102,10 +17093,10 @@
       <c r="AI74" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ74" s="43">
+      <c r="AJ74" s="42">
         <v>61363</v>
       </c>
-      <c r="AK74" s="44" t="s">
+      <c r="AK74" s="43" t="s">
         <v>215</v>
       </c>
       <c r="AL74" s="19" t="s">
@@ -17230,10 +17221,10 @@
       <c r="AI75" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ75" s="43">
+      <c r="AJ75" s="42">
         <v>61363</v>
       </c>
-      <c r="AK75" s="44" t="s">
+      <c r="AK75" s="43" t="s">
         <v>215</v>
       </c>
       <c r="AL75" s="19" t="s">
@@ -17295,7 +17286,7 @@
       <c r="AH76" s="19"/>
       <c r="AI76" s="19"/>
       <c r="AJ76" s="7"/>
-      <c r="AK76" s="40"/>
+      <c r="AK76" s="41"/>
       <c r="AL76" s="19"/>
       <c r="AM76" s="5"/>
       <c r="AN76" s="7"/>
@@ -17405,10 +17396,10 @@
       <c r="AI77" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ77" s="43">
+      <c r="AJ77" s="42">
         <v>61364</v>
       </c>
-      <c r="AK77" s="44" t="s">
+      <c r="AK77" s="43" t="s">
         <v>224</v>
       </c>
       <c r="AL77" s="19" t="s">
@@ -17533,10 +17524,10 @@
       <c r="AI78" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ78" s="43">
+      <c r="AJ78" s="42">
         <v>61364</v>
       </c>
-      <c r="AK78" s="44" t="s">
+      <c r="AK78" s="43" t="s">
         <v>224</v>
       </c>
       <c r="AL78" s="19" t="s">
@@ -17661,10 +17652,10 @@
       <c r="AI79" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ79" s="43">
+      <c r="AJ79" s="42">
         <v>61364</v>
       </c>
-      <c r="AK79" s="44" t="s">
+      <c r="AK79" s="43" t="s">
         <v>224</v>
       </c>
       <c r="AL79" s="19" t="s">
@@ -17789,10 +17780,10 @@
       <c r="AI80" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ80" s="43">
+      <c r="AJ80" s="42">
         <v>61364</v>
       </c>
-      <c r="AK80" s="44" t="s">
+      <c r="AK80" s="43" t="s">
         <v>224</v>
       </c>
       <c r="AL80" s="19" t="s">
@@ -17917,10 +17908,10 @@
       <c r="AI81" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ81" s="43">
+      <c r="AJ81" s="42">
         <v>61364</v>
       </c>
-      <c r="AK81" s="44" t="s">
+      <c r="AK81" s="43" t="s">
         <v>224</v>
       </c>
       <c r="AL81" s="19" t="s">
@@ -18045,10 +18036,10 @@
       <c r="AI82" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ82" s="43">
+      <c r="AJ82" s="42">
         <v>61364</v>
       </c>
-      <c r="AK82" s="44" t="s">
+      <c r="AK82" s="43" t="s">
         <v>224</v>
       </c>
       <c r="AL82" s="19" t="s">
@@ -18173,10 +18164,10 @@
       <c r="AI83" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ83" s="43">
+      <c r="AJ83" s="42">
         <v>61364</v>
       </c>
-      <c r="AK83" s="44" t="s">
+      <c r="AK83" s="43" t="s">
         <v>224</v>
       </c>
       <c r="AL83" s="19" t="s">
@@ -18238,7 +18229,7 @@
       <c r="AH84" s="19"/>
       <c r="AI84" s="19"/>
       <c r="AJ84" s="7"/>
-      <c r="AK84" s="40"/>
+      <c r="AK84" s="41"/>
       <c r="AL84" s="19"/>
       <c r="AM84" s="5"/>
       <c r="AN84" s="7"/>
@@ -18348,10 +18339,10 @@
       <c r="AI85" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ85" s="43">
+      <c r="AJ85" s="42">
         <v>61365</v>
       </c>
-      <c r="AK85" s="44" t="s">
+      <c r="AK85" s="43" t="s">
         <v>233</v>
       </c>
       <c r="AL85" s="19" t="s">
@@ -18476,10 +18467,10 @@
       <c r="AI86" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ86" s="43">
+      <c r="AJ86" s="42">
         <v>61365</v>
       </c>
-      <c r="AK86" s="44" t="s">
+      <c r="AK86" s="43" t="s">
         <v>233</v>
       </c>
       <c r="AL86" s="19" t="s">
@@ -18604,10 +18595,10 @@
       <c r="AI87" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ87" s="43">
+      <c r="AJ87" s="42">
         <v>61365</v>
       </c>
-      <c r="AK87" s="44" t="s">
+      <c r="AK87" s="43" t="s">
         <v>233</v>
       </c>
       <c r="AL87" s="19" t="s">
@@ -18732,10 +18723,10 @@
       <c r="AI88" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ88" s="43">
+      <c r="AJ88" s="42">
         <v>61365</v>
       </c>
-      <c r="AK88" s="44" t="s">
+      <c r="AK88" s="43" t="s">
         <v>233</v>
       </c>
       <c r="AL88" s="19" t="s">
@@ -18860,10 +18851,10 @@
       <c r="AI89" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ89" s="43">
+      <c r="AJ89" s="42">
         <v>61365</v>
       </c>
-      <c r="AK89" s="44" t="s">
+      <c r="AK89" s="43" t="s">
         <v>233</v>
       </c>
       <c r="AL89" s="19" t="s">
@@ -18988,10 +18979,10 @@
       <c r="AI90" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ90" s="43">
+      <c r="AJ90" s="42">
         <v>61365</v>
       </c>
-      <c r="AK90" s="44" t="s">
+      <c r="AK90" s="43" t="s">
         <v>233</v>
       </c>
       <c r="AL90" s="19" t="s">
@@ -19116,10 +19107,10 @@
       <c r="AI91" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ91" s="43">
+      <c r="AJ91" s="42">
         <v>61365</v>
       </c>
-      <c r="AK91" s="44" t="s">
+      <c r="AK91" s="43" t="s">
         <v>233</v>
       </c>
       <c r="AL91" s="19" t="s">
@@ -19181,7 +19172,7 @@
       <c r="AH92" s="19"/>
       <c r="AI92" s="19"/>
       <c r="AJ92" s="7"/>
-      <c r="AK92" s="40"/>
+      <c r="AK92" s="41"/>
       <c r="AL92" s="19"/>
       <c r="AM92" s="5"/>
       <c r="AN92" s="7"/>
@@ -19291,10 +19282,10 @@
       <c r="AI93" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ93" s="43">
+      <c r="AJ93" s="42">
         <v>61366</v>
       </c>
-      <c r="AK93" s="44" t="s">
+      <c r="AK93" s="43" t="s">
         <v>242</v>
       </c>
       <c r="AL93" s="19" t="s">
@@ -19419,10 +19410,10 @@
       <c r="AI94" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ94" s="43">
+      <c r="AJ94" s="42">
         <v>61366</v>
       </c>
-      <c r="AK94" s="44" t="s">
+      <c r="AK94" s="43" t="s">
         <v>242</v>
       </c>
       <c r="AL94" s="19" t="s">
@@ -19547,10 +19538,10 @@
       <c r="AI95" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ95" s="43">
+      <c r="AJ95" s="42">
         <v>61366</v>
       </c>
-      <c r="AK95" s="44" t="s">
+      <c r="AK95" s="43" t="s">
         <v>242</v>
       </c>
       <c r="AL95" s="19" t="s">
@@ -19675,10 +19666,10 @@
       <c r="AI96" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ96" s="43">
+      <c r="AJ96" s="42">
         <v>61366</v>
       </c>
-      <c r="AK96" s="44" t="s">
+      <c r="AK96" s="43" t="s">
         <v>242</v>
       </c>
       <c r="AL96" s="19" t="s">
@@ -19803,10 +19794,10 @@
       <c r="AI97" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ97" s="43">
+      <c r="AJ97" s="42">
         <v>61366</v>
       </c>
-      <c r="AK97" s="44" t="s">
+      <c r="AK97" s="43" t="s">
         <v>242</v>
       </c>
       <c r="AL97" s="19" t="s">
@@ -19931,10 +19922,10 @@
       <c r="AI98" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ98" s="43">
+      <c r="AJ98" s="42">
         <v>61366</v>
       </c>
-      <c r="AK98" s="44" t="s">
+      <c r="AK98" s="43" t="s">
         <v>242</v>
       </c>
       <c r="AL98" s="19" t="s">
@@ -20059,10 +20050,10 @@
       <c r="AI99" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ99" s="43">
+      <c r="AJ99" s="42">
         <v>61366</v>
       </c>
-      <c r="AK99" s="44" t="s">
+      <c r="AK99" s="43" t="s">
         <v>242</v>
       </c>
       <c r="AL99" s="19" t="s">
@@ -20122,7 +20113,7 @@
       <c r="AH100" s="19"/>
       <c r="AI100" s="19"/>
       <c r="AJ100" s="7"/>
-      <c r="AK100" s="40"/>
+      <c r="AK100" s="41"/>
       <c r="AL100" s="19"/>
       <c r="AM100" s="5"/>
       <c r="AN100" s="7"/>
@@ -22937,7 +22928,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="44" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">
@@ -23054,7 +23045,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="44" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">
@@ -23171,7 +23162,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="44" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">

</xml_diff>

<commit_message>
round 2 create flight
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CheckIn.xlsx
+++ b/src/main/resources/input_excel_file/booking/CheckIn.xlsx
@@ -545,7 +545,7 @@
     <t>VST_Kiểm tra check in bag khi nhập voucher giảm 10% all fee</t>
   </si>
   <si>
-    <t>CN10001</t>
+    <t>ALLFEE1</t>
   </si>
   <si>
     <t>VST_CI_VC_ALL_10_002</t>
@@ -572,7 +572,7 @@
     <t>VST_Kiểm tra check in bag khi nhập voucher giảm cố định: Green + Caddie + 1/2 xe + Package</t>
   </si>
   <si>
-    <t>CD4FEE1</t>
+    <t>CD4FEE21</t>
   </si>
   <si>
     <t>VST_CI_VC_CD4FEE_002</t>
@@ -1778,7 +1778,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1908,11 +1908,17 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
@@ -9370,7 +9376,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="47" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">
@@ -9388,10 +9394,10 @@
   <sheetPr/>
   <dimension ref="A1:AZ103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="Y1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="X1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AG23" sqref="AG23"/>
+      <selection pane="bottomLeft" activeCell="AH39" sqref="AH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -10544,7 +10550,7 @@
       <c r="AJ12" s="42">
         <v>61375</v>
       </c>
-      <c r="AK12" s="43" t="s">
+      <c r="AK12" s="40" t="s">
         <v>151</v>
       </c>
       <c r="AL12" s="19" t="s">
@@ -10650,7 +10656,7 @@
       <c r="AJ13" s="42">
         <v>61375</v>
       </c>
-      <c r="AK13" s="43" t="s">
+      <c r="AK13" s="40" t="s">
         <v>151</v>
       </c>
       <c r="AL13" s="19" t="s">
@@ -10756,7 +10762,7 @@
       <c r="AJ14" s="42">
         <v>61375</v>
       </c>
-      <c r="AK14" s="43" t="s">
+      <c r="AK14" s="40" t="s">
         <v>151</v>
       </c>
       <c r="AL14" s="19" t="s">
@@ -10862,7 +10868,7 @@
       <c r="AJ15" s="42">
         <v>61375</v>
       </c>
-      <c r="AK15" s="43" t="s">
+      <c r="AK15" s="40" t="s">
         <v>151</v>
       </c>
       <c r="AL15" s="19" t="s">
@@ -10968,7 +10974,7 @@
       <c r="AJ16" s="42">
         <v>61375</v>
       </c>
-      <c r="AK16" s="43" t="s">
+      <c r="AK16" s="40" t="s">
         <v>151</v>
       </c>
       <c r="AL16" s="19" t="s">
@@ -11074,7 +11080,7 @@
       <c r="AJ17" s="42">
         <v>61375</v>
       </c>
-      <c r="AK17" s="43" t="s">
+      <c r="AK17" s="40" t="s">
         <v>151</v>
       </c>
       <c r="AL17" s="19" t="s">
@@ -11180,7 +11186,7 @@
       <c r="AJ18" s="42">
         <v>61375</v>
       </c>
-      <c r="AK18" s="43" t="s">
+      <c r="AK18" s="40" t="s">
         <v>151</v>
       </c>
       <c r="AL18" s="19" t="s">
@@ -11333,7 +11339,7 @@
       <c r="AJ20" s="42">
         <v>61377</v>
       </c>
-      <c r="AK20" s="43" t="s">
+      <c r="AK20" s="40" t="s">
         <v>160</v>
       </c>
       <c r="AL20" s="19" t="s">
@@ -11439,7 +11445,7 @@
       <c r="AJ21" s="42">
         <v>61377</v>
       </c>
-      <c r="AK21" s="43" t="s">
+      <c r="AK21" s="40" t="s">
         <v>160</v>
       </c>
       <c r="AL21" s="19" t="s">
@@ -11545,7 +11551,7 @@
       <c r="AJ22" s="42">
         <v>61377</v>
       </c>
-      <c r="AK22" s="43" t="s">
+      <c r="AK22" s="40" t="s">
         <v>160</v>
       </c>
       <c r="AL22" s="19" t="s">
@@ -11651,7 +11657,7 @@
       <c r="AJ23" s="42">
         <v>61377</v>
       </c>
-      <c r="AK23" s="43" t="s">
+      <c r="AK23" s="40" t="s">
         <v>160</v>
       </c>
       <c r="AL23" s="19" t="s">
@@ -11757,7 +11763,7 @@
       <c r="AJ24" s="42">
         <v>61377</v>
       </c>
-      <c r="AK24" s="43" t="s">
+      <c r="AK24" s="40" t="s">
         <v>160</v>
       </c>
       <c r="AL24" s="19" t="s">
@@ -11863,7 +11869,7 @@
       <c r="AJ25" s="42">
         <v>61377</v>
       </c>
-      <c r="AK25" s="43" t="s">
+      <c r="AK25" s="40" t="s">
         <v>160</v>
       </c>
       <c r="AL25" s="19" t="s">
@@ -11969,7 +11975,7 @@
       <c r="AJ26" s="42">
         <v>61377</v>
       </c>
-      <c r="AK26" s="43" t="s">
+      <c r="AK26" s="40" t="s">
         <v>160</v>
       </c>
       <c r="AL26" s="19" t="s">
@@ -12119,10 +12125,10 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
       <c r="AI28" s="19"/>
-      <c r="AJ28" s="44">
-        <v>35540</v>
-      </c>
-      <c r="AK28" s="40" t="s">
+      <c r="AJ28" s="43">
+        <v>61378</v>
+      </c>
+      <c r="AK28" s="44" t="s">
         <v>169</v>
       </c>
       <c r="AL28" s="19" t="s">
@@ -12225,10 +12231,10 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
       <c r="AI29" s="19"/>
-      <c r="AJ29" s="44">
-        <v>35540</v>
-      </c>
-      <c r="AK29" s="40" t="s">
+      <c r="AJ29" s="43">
+        <v>61378</v>
+      </c>
+      <c r="AK29" s="44" t="s">
         <v>169</v>
       </c>
       <c r="AL29" s="19" t="s">
@@ -12331,10 +12337,10 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
       <c r="AI30" s="19"/>
-      <c r="AJ30" s="44">
-        <v>35540</v>
-      </c>
-      <c r="AK30" s="40" t="s">
+      <c r="AJ30" s="43">
+        <v>61378</v>
+      </c>
+      <c r="AK30" s="44" t="s">
         <v>169</v>
       </c>
       <c r="AL30" s="19" t="s">
@@ -12437,10 +12443,10 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
       <c r="AI31" s="19"/>
-      <c r="AJ31" s="44">
-        <v>35540</v>
-      </c>
-      <c r="AK31" s="40" t="s">
+      <c r="AJ31" s="43">
+        <v>61378</v>
+      </c>
+      <c r="AK31" s="44" t="s">
         <v>169</v>
       </c>
       <c r="AL31" s="19" t="s">
@@ -12543,10 +12549,10 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
       <c r="AI32" s="19"/>
-      <c r="AJ32" s="44">
-        <v>35540</v>
-      </c>
-      <c r="AK32" s="40" t="s">
+      <c r="AJ32" s="43">
+        <v>61378</v>
+      </c>
+      <c r="AK32" s="44" t="s">
         <v>169</v>
       </c>
       <c r="AL32" s="19" t="s">
@@ -12649,10 +12655,10 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
       <c r="AI33" s="19"/>
-      <c r="AJ33" s="44">
-        <v>35540</v>
-      </c>
-      <c r="AK33" s="40" t="s">
+      <c r="AJ33" s="43">
+        <v>61378</v>
+      </c>
+      <c r="AK33" s="44" t="s">
         <v>169</v>
       </c>
       <c r="AL33" s="19" t="s">
@@ -12755,10 +12761,10 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
       <c r="AI34" s="19"/>
-      <c r="AJ34" s="44">
-        <v>35540</v>
-      </c>
-      <c r="AK34" s="40" t="s">
+      <c r="AJ34" s="43">
+        <v>61378</v>
+      </c>
+      <c r="AK34" s="44" t="s">
         <v>169</v>
       </c>
       <c r="AL34" s="19" t="s">
@@ -12908,10 +12914,10 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
       <c r="AI36" s="19"/>
-      <c r="AJ36" s="44">
-        <v>61353</v>
-      </c>
-      <c r="AK36" s="40" t="s">
+      <c r="AJ36" s="45">
+        <v>61379</v>
+      </c>
+      <c r="AK36" s="46" t="s">
         <v>178</v>
       </c>
       <c r="AL36" s="19" t="s">
@@ -13014,10 +13020,10 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
       <c r="AI37" s="19"/>
-      <c r="AJ37" s="44">
-        <v>61353</v>
-      </c>
-      <c r="AK37" s="40" t="s">
+      <c r="AJ37" s="45">
+        <v>61379</v>
+      </c>
+      <c r="AK37" s="46" t="s">
         <v>178</v>
       </c>
       <c r="AL37" s="19" t="s">
@@ -13120,10 +13126,10 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
       <c r="AI38" s="19"/>
-      <c r="AJ38" s="44">
-        <v>61353</v>
-      </c>
-      <c r="AK38" s="40" t="s">
+      <c r="AJ38" s="45">
+        <v>61379</v>
+      </c>
+      <c r="AK38" s="46" t="s">
         <v>178</v>
       </c>
       <c r="AL38" s="19" t="s">
@@ -13226,10 +13232,10 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
       <c r="AI39" s="19"/>
-      <c r="AJ39" s="44">
-        <v>61353</v>
-      </c>
-      <c r="AK39" s="40" t="s">
+      <c r="AJ39" s="45">
+        <v>61379</v>
+      </c>
+      <c r="AK39" s="46" t="s">
         <v>178</v>
       </c>
       <c r="AL39" s="19" t="s">
@@ -13332,10 +13338,10 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
       <c r="AI40" s="19"/>
-      <c r="AJ40" s="44">
-        <v>61353</v>
-      </c>
-      <c r="AK40" s="40" t="s">
+      <c r="AJ40" s="45">
+        <v>61379</v>
+      </c>
+      <c r="AK40" s="46" t="s">
         <v>178</v>
       </c>
       <c r="AL40" s="19" t="s">
@@ -13438,10 +13444,10 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
       <c r="AI41" s="19"/>
-      <c r="AJ41" s="44">
-        <v>61353</v>
-      </c>
-      <c r="AK41" s="40" t="s">
+      <c r="AJ41" s="45">
+        <v>61379</v>
+      </c>
+      <c r="AK41" s="46" t="s">
         <v>178</v>
       </c>
       <c r="AL41" s="19" t="s">
@@ -13544,10 +13550,10 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
       <c r="AI42" s="19"/>
-      <c r="AJ42" s="44">
-        <v>61353</v>
-      </c>
-      <c r="AK42" s="40" t="s">
+      <c r="AJ42" s="45">
+        <v>61379</v>
+      </c>
+      <c r="AK42" s="46" t="s">
         <v>178</v>
       </c>
       <c r="AL42" s="19" t="s">
@@ -13697,7 +13703,7 @@
       <c r="AG44" s="19"/>
       <c r="AH44" s="19"/>
       <c r="AI44" s="19"/>
-      <c r="AJ44" s="44">
+      <c r="AJ44" s="42">
         <v>61357</v>
       </c>
       <c r="AK44" s="40" t="s">
@@ -13803,7 +13809,7 @@
       <c r="AG45" s="19"/>
       <c r="AH45" s="19"/>
       <c r="AI45" s="19"/>
-      <c r="AJ45" s="44">
+      <c r="AJ45" s="42">
         <v>61357</v>
       </c>
       <c r="AK45" s="40" t="s">
@@ -13909,7 +13915,7 @@
       <c r="AG46" s="19"/>
       <c r="AH46" s="19"/>
       <c r="AI46" s="19"/>
-      <c r="AJ46" s="44">
+      <c r="AJ46" s="42">
         <v>61357</v>
       </c>
       <c r="AK46" s="40" t="s">
@@ -14015,7 +14021,7 @@
       <c r="AG47" s="19"/>
       <c r="AH47" s="19"/>
       <c r="AI47" s="19"/>
-      <c r="AJ47" s="44">
+      <c r="AJ47" s="42">
         <v>61357</v>
       </c>
       <c r="AK47" s="40" t="s">
@@ -14121,7 +14127,7 @@
       <c r="AG48" s="19"/>
       <c r="AH48" s="19"/>
       <c r="AI48" s="19"/>
-      <c r="AJ48" s="44">
+      <c r="AJ48" s="42">
         <v>61357</v>
       </c>
       <c r="AK48" s="40" t="s">
@@ -14227,7 +14233,7 @@
       <c r="AG49" s="19"/>
       <c r="AH49" s="19"/>
       <c r="AI49" s="19"/>
-      <c r="AJ49" s="44">
+      <c r="AJ49" s="42">
         <v>61357</v>
       </c>
       <c r="AK49" s="40" t="s">
@@ -14333,7 +14339,7 @@
       <c r="AG50" s="19"/>
       <c r="AH50" s="19"/>
       <c r="AI50" s="19"/>
-      <c r="AJ50" s="44">
+      <c r="AJ50" s="42">
         <v>61357</v>
       </c>
       <c r="AK50" s="40" t="s">
@@ -14564,7 +14570,7 @@
       <c r="AI53" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ53" s="44">
+      <c r="AJ53" s="42">
         <v>61361</v>
       </c>
       <c r="AK53" s="40" t="s">
@@ -14693,7 +14699,7 @@
       <c r="AI54" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ54" s="44">
+      <c r="AJ54" s="42">
         <v>61361</v>
       </c>
       <c r="AK54" s="40" t="s">
@@ -14822,7 +14828,7 @@
       <c r="AI55" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ55" s="44">
+      <c r="AJ55" s="42">
         <v>61361</v>
       </c>
       <c r="AK55" s="40" t="s">
@@ -14951,7 +14957,7 @@
       <c r="AI56" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ56" s="44">
+      <c r="AJ56" s="42">
         <v>61361</v>
       </c>
       <c r="AK56" s="40" t="s">
@@ -15080,7 +15086,7 @@
       <c r="AI57" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ57" s="44">
+      <c r="AJ57" s="42">
         <v>61361</v>
       </c>
       <c r="AK57" s="40" t="s">
@@ -15209,7 +15215,7 @@
       <c r="AI58" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ58" s="44">
+      <c r="AJ58" s="42">
         <v>61361</v>
       </c>
       <c r="AK58" s="40" t="s">
@@ -15338,7 +15344,7 @@
       <c r="AI59" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ59" s="44">
+      <c r="AJ59" s="42">
         <v>61361</v>
       </c>
       <c r="AK59" s="40" t="s">
@@ -15513,7 +15519,7 @@
       <c r="AI61" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ61" s="44">
+      <c r="AJ61" s="42">
         <v>61362</v>
       </c>
       <c r="AK61" s="40" t="s">
@@ -15641,7 +15647,7 @@
       <c r="AI62" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ62" s="44">
+      <c r="AJ62" s="42">
         <v>61362</v>
       </c>
       <c r="AK62" s="40" t="s">
@@ -15769,7 +15775,7 @@
       <c r="AI63" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ63" s="44">
+      <c r="AJ63" s="42">
         <v>61362</v>
       </c>
       <c r="AK63" s="40" t="s">
@@ -15897,7 +15903,7 @@
       <c r="AI64" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ64" s="44">
+      <c r="AJ64" s="42">
         <v>61362</v>
       </c>
       <c r="AK64" s="40" t="s">
@@ -16025,7 +16031,7 @@
       <c r="AI65" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ65" s="44">
+      <c r="AJ65" s="42">
         <v>61362</v>
       </c>
       <c r="AK65" s="40" t="s">
@@ -16153,7 +16159,7 @@
       <c r="AI66" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ66" s="44">
+      <c r="AJ66" s="42">
         <v>61362</v>
       </c>
       <c r="AK66" s="40" t="s">
@@ -16281,7 +16287,7 @@
       <c r="AI67" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ67" s="44">
+      <c r="AJ67" s="42">
         <v>61362</v>
       </c>
       <c r="AK67" s="40" t="s">
@@ -16456,7 +16462,7 @@
       <c r="AI69" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ69" s="44">
+      <c r="AJ69" s="42">
         <v>61363</v>
       </c>
       <c r="AK69" s="40" t="s">
@@ -16584,7 +16590,7 @@
       <c r="AI70" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ70" s="44">
+      <c r="AJ70" s="42">
         <v>61363</v>
       </c>
       <c r="AK70" s="40" t="s">
@@ -16712,7 +16718,7 @@
       <c r="AI71" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ71" s="44">
+      <c r="AJ71" s="42">
         <v>61363</v>
       </c>
       <c r="AK71" s="40" t="s">
@@ -16840,7 +16846,7 @@
       <c r="AI72" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ72" s="44">
+      <c r="AJ72" s="42">
         <v>61363</v>
       </c>
       <c r="AK72" s="40" t="s">
@@ -16968,7 +16974,7 @@
       <c r="AI73" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ73" s="44">
+      <c r="AJ73" s="42">
         <v>61363</v>
       </c>
       <c r="AK73" s="40" t="s">
@@ -17096,7 +17102,7 @@
       <c r="AI74" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ74" s="44">
+      <c r="AJ74" s="42">
         <v>61363</v>
       </c>
       <c r="AK74" s="40" t="s">
@@ -17224,7 +17230,7 @@
       <c r="AI75" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ75" s="44">
+      <c r="AJ75" s="42">
         <v>61363</v>
       </c>
       <c r="AK75" s="40" t="s">
@@ -17399,7 +17405,7 @@
       <c r="AI77" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ77" s="44">
+      <c r="AJ77" s="42">
         <v>61364</v>
       </c>
       <c r="AK77" s="40" t="s">
@@ -17527,7 +17533,7 @@
       <c r="AI78" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ78" s="44">
+      <c r="AJ78" s="42">
         <v>61364</v>
       </c>
       <c r="AK78" s="40" t="s">
@@ -17655,7 +17661,7 @@
       <c r="AI79" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ79" s="44">
+      <c r="AJ79" s="42">
         <v>61364</v>
       </c>
       <c r="AK79" s="40" t="s">
@@ -17783,7 +17789,7 @@
       <c r="AI80" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ80" s="44">
+      <c r="AJ80" s="42">
         <v>61364</v>
       </c>
       <c r="AK80" s="40" t="s">
@@ -17911,7 +17917,7 @@
       <c r="AI81" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ81" s="44">
+      <c r="AJ81" s="42">
         <v>61364</v>
       </c>
       <c r="AK81" s="40" t="s">
@@ -18039,7 +18045,7 @@
       <c r="AI82" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ82" s="44">
+      <c r="AJ82" s="42">
         <v>61364</v>
       </c>
       <c r="AK82" s="40" t="s">
@@ -18167,7 +18173,7 @@
       <c r="AI83" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ83" s="44">
+      <c r="AJ83" s="42">
         <v>61364</v>
       </c>
       <c r="AK83" s="40" t="s">
@@ -18342,7 +18348,7 @@
       <c r="AI85" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ85" s="44">
+      <c r="AJ85" s="42">
         <v>61365</v>
       </c>
       <c r="AK85" s="40" t="s">
@@ -18470,7 +18476,7 @@
       <c r="AI86" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ86" s="44">
+      <c r="AJ86" s="42">
         <v>61365</v>
       </c>
       <c r="AK86" s="40" t="s">
@@ -18598,7 +18604,7 @@
       <c r="AI87" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ87" s="44">
+      <c r="AJ87" s="42">
         <v>61365</v>
       </c>
       <c r="AK87" s="40" t="s">
@@ -18726,7 +18732,7 @@
       <c r="AI88" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ88" s="44">
+      <c r="AJ88" s="42">
         <v>61365</v>
       </c>
       <c r="AK88" s="40" t="s">
@@ -18854,7 +18860,7 @@
       <c r="AI89" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ89" s="44">
+      <c r="AJ89" s="42">
         <v>61365</v>
       </c>
       <c r="AK89" s="40" t="s">
@@ -18982,7 +18988,7 @@
       <c r="AI90" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ90" s="44">
+      <c r="AJ90" s="42">
         <v>61365</v>
       </c>
       <c r="AK90" s="40" t="s">
@@ -19110,7 +19116,7 @@
       <c r="AI91" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ91" s="44">
+      <c r="AJ91" s="42">
         <v>61365</v>
       </c>
       <c r="AK91" s="40" t="s">
@@ -19285,7 +19291,7 @@
       <c r="AI93" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ93" s="44">
+      <c r="AJ93" s="42">
         <v>61366</v>
       </c>
       <c r="AK93" s="40" t="s">
@@ -19413,7 +19419,7 @@
       <c r="AI94" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ94" s="44">
+      <c r="AJ94" s="42">
         <v>61366</v>
       </c>
       <c r="AK94" s="40" t="s">
@@ -19541,7 +19547,7 @@
       <c r="AI95" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ95" s="44">
+      <c r="AJ95" s="42">
         <v>61366</v>
       </c>
       <c r="AK95" s="40" t="s">
@@ -19669,7 +19675,7 @@
       <c r="AI96" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ96" s="44">
+      <c r="AJ96" s="42">
         <v>61366</v>
       </c>
       <c r="AK96" s="40" t="s">
@@ -19797,7 +19803,7 @@
       <c r="AI97" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ97" s="44">
+      <c r="AJ97" s="42">
         <v>61366</v>
       </c>
       <c r="AK97" s="40" t="s">
@@ -19925,7 +19931,7 @@
       <c r="AI98" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ98" s="44">
+      <c r="AJ98" s="42">
         <v>61366</v>
       </c>
       <c r="AK98" s="40" t="s">
@@ -20053,7 +20059,7 @@
       <c r="AI99" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AJ99" s="44">
+      <c r="AJ99" s="42">
         <v>61366</v>
       </c>
       <c r="AK99" s="40" t="s">
@@ -22931,7 +22937,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="47" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">
@@ -23048,7 +23054,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="47" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">
@@ -23165,7 +23171,7 @@
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="47" t="s">
         <v>316</v>
       </c>
       <c r="M2" s="7" t="s">

</xml_diff>